<commit_message>
address and kadastr del from name
</commit_message>
<xml_diff>
--- a/torgi/output.xlsx
+++ b/torgi/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P29"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,72 +441,47 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>Регион</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Общая площадь</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Название</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Цена</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Окончания подачи заявок</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Кадастровый номер</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Кадастровая стоимость</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Форма проведения</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
           <t>Имущество</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Форма проведения</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Название</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Цена</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Окончания подачи заявок</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Общая площадь</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Общие сведения об ограничениях и обременениях </t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Вид ограничений и обременений</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Назначение нежилого помещения</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Кадастровый номер объекта недвижимости (здания, сооружения), в пределах которого расположено помещение</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Кадастровый номер</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Кадастровая стоимость </t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>Расположение в пределах объекта недвижимости (этажа, части этажа, нескольких этажей)</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>Год ввода в эксплуатацию</t>
         </is>
       </c>
     </row>
@@ -521,17 +496,15 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Должников</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>EA</t>
-        </is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>283.2</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>нежилое помещение, площадью 283,20 кв. м, расположенное по адресу: Чувашская Республика, п. Ибреси, ул. СХТ, д. 24, кадастровый № 21:10:000000:1355</t>
+          <t xml:space="preserve">нежилое помещение, площадью 283,20 кв. м, </t>
         </is>
       </c>
       <c r="F2" t="n">
@@ -542,37 +515,22 @@
           <t>08/07/22 17:00</t>
         </is>
       </c>
-      <c r="H2" t="n">
-        <v>283.2</v>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>арестованное, наличие ограничений: запрет на регистрационные действия</t>
-        </is>
-      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>21:10:000000:1355</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr">
         <is>
-          <t>арестованное, наличие ограничений: запрет на регистрационные действия</t>
+          <t>EA</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>нежилое помещение</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>21:10:000000:1355</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>21:10:000000:1355</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr"/>
-      <c r="O2" t="inlineStr"/>
-      <c r="P2" t="inlineStr"/>
+          <t>Должников</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -585,17 +543,15 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Должников</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>EA</t>
-        </is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>1227.3</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>здание нежилое площадью 1227,30 кв. м, расположенное по адресу: Чувашская Республика, Ибресинский район, п. Буинск, ул. Заводская, д. 20, кадастровый № 21:10:200110:155</t>
+          <t xml:space="preserve">здание нежилое площадью 1227,30 кв. м, </t>
         </is>
       </c>
       <c r="F3" t="n">
@@ -606,37 +562,22 @@
           <t>08/07/22 17:00</t>
         </is>
       </c>
-      <c r="H3" t="n">
-        <v>1227.3</v>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>арестованное, наличие ограничений: запрет на регистрационные действия</t>
-        </is>
-      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>21:10:200110:155</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr">
         <is>
-          <t>арестованное, наличие ограничений: запрет на регистрационные действия</t>
+          <t>EA</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t xml:space="preserve">здание нежилое </t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>21:10:200110:155</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>21:10:200110:155</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr"/>
-      <c r="P3" t="inlineStr"/>
+          <t>Должников</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -649,17 +590,15 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Должников</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>EA</t>
-        </is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>310.9</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>здание нежилое площадью 310,90 кв. м, расположенное по адресу: Чувашская Республика, Ибресинский район, п. Буинск, ул. Заводская, д. 20, кадастровый № 21:10:200110:121</t>
+          <t xml:space="preserve">здание нежилое площадью 310,90 кв. м, </t>
         </is>
       </c>
       <c r="F4" t="n">
@@ -670,37 +609,22 @@
           <t>08/07/22 17:00</t>
         </is>
       </c>
-      <c r="H4" t="n">
-        <v>310.9</v>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>арестованное, наличие ограничений: запрет на регистрационные действия</t>
-        </is>
-      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>21:10:200110:121</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr">
         <is>
-          <t>арестованное, наличие ограничений: запрет на регистрационные действия</t>
+          <t>EA</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t xml:space="preserve">здание нежилое </t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>21:10:200110:121</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>21:10:200110:121</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr"/>
-      <c r="O4" t="inlineStr"/>
-      <c r="P4" t="inlineStr"/>
+          <t>Должников</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -713,17 +637,15 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Муниципальное</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>PP</t>
-        </is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>401.1</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Муниципальное имущество Яльчикского района</t>
+          <t xml:space="preserve">Муниципальное имущество Яльчикского района, </t>
         </is>
       </c>
       <c r="F5" t="n">
@@ -734,37 +656,22 @@
           <t>05/07/22 20:30</t>
         </is>
       </c>
-      <c r="H5" t="n">
-        <v>401.1</v>
-      </c>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr"/>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>21:25:180308:517</t>
+        </is>
+      </c>
+      <c r="I5" t="n">
+        <v>302518043</v>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>PP</t>
+        </is>
+      </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>административное</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>21:25:180310:90</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>21:25:180308:517</t>
-        </is>
-      </c>
-      <c r="N5" t="n">
-        <v>302518043</v>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>1 и 2 этаж</t>
-        </is>
-      </c>
-      <c r="P5" t="inlineStr">
-        <is>
-          <t>1969</t>
+          <t>Муниципальное</t>
         </is>
       </c>
     </row>
@@ -779,17 +686,15 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Муниципальное</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>PP</t>
-        </is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>676.4</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Помещение, назначение: нежилое, общая площадь - 676,4 кв. м, этаж 1, номера на поэтажном плане поз. 1 - 13, 15 - 22, кадастровый номер: 12:05:0000000:12935, местоположение: Республика Марий Эл, г. Йошкар-Ола, ул. Красноармейская, д. 103а</t>
+          <t xml:space="preserve">Помещение, назначение: нежилое, общая площадь - 676,4 кв. м, этаж 1, номера на поэтажном плане поз. 1 - 13, 15 - 22, </t>
         </is>
       </c>
       <c r="F6" t="n">
@@ -800,27 +705,22 @@
           <t>11/07/22 14:30</t>
         </is>
       </c>
-      <c r="H6" t="n">
-        <v>676.4</v>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Имущество в споре или под арестом не состоит, не является предметом залога 
-и не обременено другими правами третьих лиц. 
- </t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 12:05:0000000:12935</t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr"/>
-      <c r="N6" t="inlineStr"/>
-      <c r="O6" t="inlineStr"/>
-      <c r="P6" t="inlineStr"/>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>12:05:0000000:12935</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>PP</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>Муниципальное</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -833,17 +733,15 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Должников</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>EA</t>
-        </is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>76.59999999999999</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Нежилое помещение площадью 76,6 кв.м., кад. № 12:04:0270104:71 с земельным участком (для размещения хозяйственного магазина) площадью 264 кв.м., кад. № 12:04:0270104:2, расположены по адресу: РМЭ, Медведевский район, с. Азаново, ул. Советская, д.13А, принадлежащие ПК «Медведевское райпо»</t>
+          <t xml:space="preserve">Нежилое помещение площадью 76,6 кв.м. с земельным участком (для размещения хозяйственного магазина) площадью 264 кв.м., </t>
         </is>
       </c>
       <c r="F7" t="n">
@@ -854,39 +752,20 @@
           <t>11/07/22 14:00</t>
         </is>
       </c>
-      <c r="H7" t="n">
-        <v>76.59999999999999</v>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>12:04:0270104:71</t>
+        </is>
       </c>
       <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr">
         <is>
-          <t>Арест</t>
+          <t>EA</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t xml:space="preserve">12:04:0270104:71 </t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr"/>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="P7" t="inlineStr">
-        <is>
-          <t>-</t>
+          <t>Должников</t>
         </is>
       </c>
     </row>
@@ -901,17 +780,15 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Должников</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>EA</t>
-        </is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>81.09999999999999</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Нежилое помещение площадью 81,1 кв.м., кад. № 12:04:0261801:11, расположено по адресу: РМЭ, Медведевский район, п. Сурок, ул. Мира, д.4, принадлежащее ПК «Медведевское райпо».</t>
+          <t xml:space="preserve">Нежилое помещение площадью 81,1 кв.м., </t>
         </is>
       </c>
       <c r="F8" t="n">
@@ -922,35 +799,20 @@
           <t>11/07/22 14:00</t>
         </is>
       </c>
-      <c r="H8" t="n">
-        <v>81.09999999999999</v>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>12:04:0261801:11</t>
+        </is>
       </c>
       <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Арест</t>
+          <t>EA</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr"/>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>12:04:0261801:11</t>
-        </is>
-      </c>
-      <c r="N8" t="inlineStr"/>
-      <c r="O8" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="P8" t="inlineStr">
-        <is>
-          <t>-</t>
+          <t>Должников</t>
         </is>
       </c>
     </row>
@@ -965,17 +827,15 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Должников</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>EA</t>
-        </is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>6.2</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1/2 доли в праве общей долевой собственности на нежилое помещение, площадью 6,20 кв. м, находящееся по адресу: Чувашская Республика, г. Чебоксары, ул. Э. М. Юрьева, д. 10, пом. 25, кадастровый номер 21:01:010102:462</t>
+          <t xml:space="preserve">1/2 доли в праве общей долевой собственности на нежилое помещение, площадью 6,20 кв. м, </t>
         </is>
       </c>
       <c r="F9" t="n">
@@ -986,25 +846,22 @@
           <t>19/07/22 14:00</t>
         </is>
       </c>
-      <c r="H9" t="n">
-        <v>6.2</v>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>21:01:010102:462</t>
+        </is>
       </c>
       <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>21:01:010102:462</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>21:01:010102:462</t>
-        </is>
-      </c>
-      <c r="N9" t="inlineStr"/>
-      <c r="O9" t="inlineStr"/>
-      <c r="P9" t="inlineStr"/>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>EA</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>Должников</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -1017,17 +874,15 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Должников</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>EA</t>
-        </is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>20.1</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>нежилое помещение, площадью 20,10 кв. м, расположенное по адресу: Чувашская Республика, г. Новочебоксарск, ул. Строителей, владение 33А, многоэтажная автостоянка  с сервисным обслуживанием, гаражный бокс №71, кадастровый номер 21:02:010510:2846</t>
+          <t xml:space="preserve">нежилое помещение, площадью 20,10 кв. м, </t>
         </is>
       </c>
       <c r="F10" t="n">
@@ -1038,25 +893,22 @@
           <t>13/07/22 14:00</t>
         </is>
       </c>
-      <c r="H10" t="n">
-        <v>20.1</v>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>21:02:010510:2846</t>
+        </is>
       </c>
       <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>21:02:010510:2846</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>21:02:010510:2846</t>
-        </is>
-      </c>
-      <c r="N10" t="inlineStr"/>
-      <c r="O10" t="inlineStr"/>
-      <c r="P10" t="inlineStr"/>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>EA</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>Должников</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -1069,17 +921,15 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Должников</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>EA</t>
-        </is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>20.6</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Нежилое помещение, площадью 20,60 кв. м, расположенное по адресу: Чувашская Республика, г. Новочебоксарск, ул. Строителей, вл. 33А, многоэтажная автостоянка с сервисным обслуживанием, гаражный бокс № 68, кадастровый номер 21:02:010510:2854</t>
+          <t xml:space="preserve">Нежилое помещение, площадью 20,60 кв. м, </t>
         </is>
       </c>
       <c r="F11" t="n">
@@ -1090,25 +940,22 @@
           <t>19/07/22 14:00</t>
         </is>
       </c>
-      <c r="H11" t="n">
-        <v>20.6</v>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>21:02:010510:2854</t>
+        </is>
       </c>
       <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr"/>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>21:02:010510:2854</t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>21:02:010510:2854</t>
-        </is>
-      </c>
-      <c r="N11" t="inlineStr"/>
-      <c r="O11" t="inlineStr"/>
-      <c r="P11" t="inlineStr"/>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>EA</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>Должников</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -1121,17 +968,15 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Должников</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>EA</t>
-        </is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>6.2</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>1/2 доли в праве общей долевой собственности на нежилое помещение, площадью 6,20 кв. м, находящееся по адресу: Чувашская Республика, г. Чебоксары, ул. Э. М. Юрьева, д. 10, пом. 25, кадастровый номер 21:01:010102:462</t>
+          <t xml:space="preserve">1/2 доли в праве общей долевой собственности на нежилое помещение, площадью 6,20 кв. м, </t>
         </is>
       </c>
       <c r="F12" t="n">
@@ -1142,25 +987,22 @@
           <t>19/07/22 14:00</t>
         </is>
       </c>
-      <c r="H12" t="n">
-        <v>6.2</v>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>21:01:010102:462</t>
+        </is>
       </c>
       <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr"/>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>21:01:010102:462</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>21:01:010102:462</t>
-        </is>
-      </c>
-      <c r="N12" t="inlineStr"/>
-      <c r="O12" t="inlineStr"/>
-      <c r="P12" t="inlineStr"/>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>EA</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>Должников</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -1173,17 +1015,15 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Должников</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>EA</t>
-        </is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>1382.5</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>нежилое здание, картофелехранилище, площадью 1382,5 кв. м, расположенное по адресу: Чувашская Республика, Красночетайский район, с. Пандиково, кадастровый № 21:15:000000:947</t>
+          <t xml:space="preserve">нежилое здание, картофелехранилище, площадью 1382,5 кв. м, </t>
         </is>
       </c>
       <c r="F13" t="n">
@@ -1194,25 +1034,22 @@
           <t>13/07/22 14:00</t>
         </is>
       </c>
-      <c r="H13" t="n">
-        <v>1382.5</v>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>21:15:000000:947</t>
+        </is>
       </c>
       <c r="I13" t="inlineStr"/>
-      <c r="J13" t="inlineStr"/>
-      <c r="K13" t="inlineStr"/>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>21:15:000000:947</t>
-        </is>
-      </c>
-      <c r="M13" t="inlineStr">
-        <is>
-          <t>21:15:000000:947</t>
-        </is>
-      </c>
-      <c r="N13" t="inlineStr"/>
-      <c r="O13" t="inlineStr"/>
-      <c r="P13" t="inlineStr"/>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>EA</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>Должников</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -1225,17 +1062,15 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Должников</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>EA</t>
-        </is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>6.2</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>помещение нежилое, площадью 6,2 кв. м, расположенное по адресу: Чувашская Республика, г. Новочебоксарск, ул. 10 Пятилетки, д. 5А, пом. 3, кадастровый № 21:02:010223:2348</t>
+          <t xml:space="preserve">помещение нежилое, площадью 6,2 кв. м, </t>
         </is>
       </c>
       <c r="F14" t="n">
@@ -1246,25 +1081,22 @@
           <t>13/07/22 14:00</t>
         </is>
       </c>
-      <c r="H14" t="n">
-        <v>6.2</v>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>21:02:010223:2348</t>
+        </is>
       </c>
       <c r="I14" t="inlineStr"/>
-      <c r="J14" t="inlineStr"/>
-      <c r="K14" t="inlineStr"/>
-      <c r="L14" t="inlineStr">
-        <is>
-          <t>21:02:010223:2348</t>
-        </is>
-      </c>
-      <c r="M14" t="inlineStr">
-        <is>
-          <t>21:02:010223:2348</t>
-        </is>
-      </c>
-      <c r="N14" t="inlineStr"/>
-      <c r="O14" t="inlineStr"/>
-      <c r="P14" t="inlineStr"/>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>EA</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>Должников</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -1277,17 +1109,15 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Должников</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>EA</t>
-        </is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>222.2</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>здание нежилое площадью 222,20 кв. м, расположенное по адресу: Чувашская Республика, Ибресинский район, п. Буинск, ул. Заводская, д. 20, кадастровый № 21:10:200110:141</t>
+          <t xml:space="preserve">здание нежилое площадью 222,20 кв. м, </t>
         </is>
       </c>
       <c r="F15" t="n">
@@ -1298,37 +1128,22 @@
           <t>08/07/22 17:00</t>
         </is>
       </c>
-      <c r="H15" t="n">
-        <v>222.2</v>
-      </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>арестованное, наличие ограничений: запрет на регистрационные действия</t>
-        </is>
-      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>21:10:200110:141</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr"/>
       <c r="J15" t="inlineStr">
         <is>
-          <t>арестованное, наличие ограничений: запрет на регистрационные действия</t>
+          <t>EA</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>здание нежилое площадью</t>
-        </is>
-      </c>
-      <c r="L15" t="inlineStr">
-        <is>
-          <t>21:10:200110:141</t>
-        </is>
-      </c>
-      <c r="M15" t="inlineStr">
-        <is>
-          <t>21:10:200110:141</t>
-        </is>
-      </c>
-      <c r="N15" t="inlineStr"/>
-      <c r="O15" t="inlineStr"/>
-      <c r="P15" t="inlineStr"/>
+          <t>Должников</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -1341,17 +1156,15 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Должников</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>EA</t>
-        </is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>512.1</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>здание нежилое площадью 512,10 кв. м, расположенное по адресу: Чувашская Республика, Ибресинский район, п. Буинск, ул. Заводская, д. 20, кадастровый № 21:10:200110:153</t>
+          <t xml:space="preserve">здание нежилое площадью 512,10 кв. м, </t>
         </is>
       </c>
       <c r="F16" t="n">
@@ -1362,37 +1175,22 @@
           <t>08/07/22 17:00</t>
         </is>
       </c>
-      <c r="H16" t="n">
-        <v>512.1</v>
-      </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>арестованное, наличие ограничений: запрет на регистрационные действия</t>
-        </is>
-      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>21:10:200110:153</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr"/>
       <c r="J16" t="inlineStr">
         <is>
-          <t>арестованное, наличие ограничений: запрет на регистрационные действия</t>
+          <t>EA</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t xml:space="preserve">Лот №5.	здание нежилое площадью </t>
-        </is>
-      </c>
-      <c r="L16" t="inlineStr">
-        <is>
-          <t>21:10:200110:153</t>
-        </is>
-      </c>
-      <c r="M16" t="inlineStr">
-        <is>
-          <t>21:10:200110:153</t>
-        </is>
-      </c>
-      <c r="N16" t="inlineStr"/>
-      <c r="O16" t="inlineStr"/>
-      <c r="P16" t="inlineStr"/>
+          <t>Должников</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -1405,17 +1203,15 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Муниципальное</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>EA</t>
-        </is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>237.4</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Нежилое помещение, назначение: нежилое, количество этажей - 1, площадь - 237,4 кв. м, инвентарный N Р19/450-3-н, расположенное по адресу: Чувашская Республика - Чувашия, р-н Урмарский, д. Саруй, ул. Молодежная, д. 2а, пом. 2, кадастровый номер 21:19:110301:628</t>
+          <t xml:space="preserve">Нежилое помещение, назначение: нежилое, количество этажей - 1, площадь - 237,4 кв. м, инвентарный N Р19/450-3-н, </t>
         </is>
       </c>
       <c r="F17" t="n">
@@ -1426,29 +1222,22 @@
           <t>17/07/22 17:00</t>
         </is>
       </c>
-      <c r="H17" t="n">
-        <v>237.4</v>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>21:19:110301:628</t>
+        </is>
       </c>
       <c r="I17" t="inlineStr"/>
-      <c r="J17" t="inlineStr"/>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>EA</t>
+        </is>
+      </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>нежилое помещение</t>
-        </is>
-      </c>
-      <c r="L17" t="inlineStr">
-        <is>
-          <t>21:19:110301:628</t>
-        </is>
-      </c>
-      <c r="M17" t="inlineStr"/>
-      <c r="N17" t="inlineStr"/>
-      <c r="O17" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="P17" t="inlineStr"/>
+          <t>Муниципальное</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -1461,17 +1250,15 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Муниципальное</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>EA</t>
-        </is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>473.7</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Нежилое помещение, помещение 2б, расположенное на первом этаже двухэтажного кир-пичного нежилого здания, площадь ОКС’а 117,20 кв.м., кадастровый №21:19:170103:2962,Нежилое помещение, помещение 2в, расположенное на первом и втором этажах двухэтажного кирпичного нежилого здания, площадь ОКС’а 77,20 кв.м., кадастровый №21:19:170103:2964,Нежилое помещение, помещение 2г, расположенное на втором этаже двухэтажного кирпичного нежилого здания, площадь ОКС’а 279,30 кв.м., кадастровый №21:19:170103:2963</t>
+          <t>Нежилое помещение, помещение 2б, расположенное на первом этаже двухэтажного кир-пичного нежилого здания, площадь ОКС’а 117,20 кв.м.,Нежилое п</t>
         </is>
       </c>
       <c r="F18" t="n">
@@ -1482,21 +1269,22 @@
           <t>17/07/22 17:00</t>
         </is>
       </c>
-      <c r="H18" t="n">
-        <v>473.7</v>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>21:19:170103:2962</t>
+        </is>
       </c>
       <c r="I18" t="inlineStr"/>
-      <c r="J18" t="inlineStr"/>
-      <c r="K18" t="inlineStr"/>
-      <c r="L18" t="inlineStr"/>
-      <c r="M18" t="inlineStr"/>
-      <c r="N18" t="inlineStr"/>
-      <c r="O18" t="inlineStr">
-        <is>
-          <t>1-2</t>
-        </is>
-      </c>
-      <c r="P18" t="inlineStr"/>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>EA</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>Муниципальное</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -1509,17 +1297,15 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Муниципальное</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>PP</t>
-        </is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>2121.6</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Муниципальное имущество Яльчикского района, расположенное по адресу: Чувашская Республика-Чувашия, Яльчикский р-н, с Новое Тинчурино, ул Пришкольная, д 41, пом 1</t>
+          <t xml:space="preserve">Муниципальное имущество Яльчикского района, </t>
         </is>
       </c>
       <c r="F19" t="n">
@@ -1530,37 +1316,22 @@
           <t>05/07/22 20:30</t>
         </is>
       </c>
-      <c r="H19" t="n">
-        <v>2121.6</v>
-      </c>
-      <c r="I19" t="inlineStr"/>
-      <c r="J19" t="inlineStr"/>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>21:25:060402:249</t>
+        </is>
+      </c>
+      <c r="I19" t="n">
+        <v>1905322866</v>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>PP</t>
+        </is>
+      </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>административное</t>
-        </is>
-      </c>
-      <c r="L19" t="inlineStr">
-        <is>
-          <t>21:25:060402:82</t>
-        </is>
-      </c>
-      <c r="M19" t="inlineStr">
-        <is>
-          <t>21:25:060402:249</t>
-        </is>
-      </c>
-      <c r="N19" t="n">
-        <v>1905322866</v>
-      </c>
-      <c r="O19" t="inlineStr">
-        <is>
-          <t>1 и 2 этаж</t>
-        </is>
-      </c>
-      <c r="P19" t="inlineStr">
-        <is>
-          <t>1975</t>
+          <t>Муниципальное</t>
         </is>
       </c>
     </row>
@@ -1575,17 +1346,15 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Должников</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>EA</t>
-        </is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>20.2</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Нежилое помещение, площадью 20,20 кв. м, расположенное по адресу: Чувашская Республика, г. Новочебоксарск, гаражный кооператив № 7 "Прогресс", гараж-бокс № 665, кадастровый номер 21:02:010905:1073</t>
+          <t xml:space="preserve">Нежилое помещение, площадью 20,20 кв. м, </t>
         </is>
       </c>
       <c r="F20" t="n">
@@ -1596,25 +1365,22 @@
           <t>13/07/22 14:00</t>
         </is>
       </c>
-      <c r="H20" t="n">
-        <v>20.2</v>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>21:02:010905:1073</t>
+        </is>
       </c>
       <c r="I20" t="inlineStr"/>
-      <c r="J20" t="inlineStr"/>
-      <c r="K20" t="inlineStr"/>
-      <c r="L20" t="inlineStr">
-        <is>
-          <t>21:02:010905:1073</t>
-        </is>
-      </c>
-      <c r="M20" t="inlineStr">
-        <is>
-          <t>21:02:010905:1073</t>
-        </is>
-      </c>
-      <c r="N20" t="inlineStr"/>
-      <c r="O20" t="inlineStr"/>
-      <c r="P20" t="inlineStr"/>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>EA</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>Должников</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -1627,17 +1393,15 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Должников</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>EA</t>
-        </is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>2.5</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>1/2 доля в праве общей долевой собственности на нежилое помещение (кладовая), площадью 2,50 кв. м, расположенное по адресу: Чувашская Республика, г. Чебоксары, проспект Тракторостроителей, д. 34, корпус 1, хозяйственная кладовая № 19, кадастровый номер 21:01:030407:7173</t>
+          <t xml:space="preserve">1/2 доля в праве общей долевой собственности на нежилое помещение (кладовая), площадью 2,50 кв. м, </t>
         </is>
       </c>
       <c r="F21" t="n">
@@ -1648,25 +1412,22 @@
           <t>13/07/22 14:00</t>
         </is>
       </c>
-      <c r="H21" t="n">
-        <v>2.5</v>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>21:01:030407:7173</t>
+        </is>
       </c>
       <c r="I21" t="inlineStr"/>
-      <c r="J21" t="inlineStr"/>
-      <c r="K21" t="inlineStr"/>
-      <c r="L21" t="inlineStr">
-        <is>
-          <t>21:01:030407:7173</t>
-        </is>
-      </c>
-      <c r="M21" t="inlineStr">
-        <is>
-          <t>21:01:030407:7173</t>
-        </is>
-      </c>
-      <c r="N21" t="inlineStr"/>
-      <c r="O21" t="inlineStr"/>
-      <c r="P21" t="inlineStr"/>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>EA</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>Должников</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -1679,17 +1440,15 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Должников</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>EA</t>
-        </is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>271.2</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>здание нежилое площадью 271,20 кв. м, расположенное по адресу: Чувашская Республика, Ибресинский район, п. Буинск, ул. Заводская, д. 20, кадастровый № 21:10:200110:159</t>
+          <t xml:space="preserve">здание нежилое площадью 271,20 кв. м, </t>
         </is>
       </c>
       <c r="F22" t="n">
@@ -1700,37 +1459,22 @@
           <t>08/07/22 17:00</t>
         </is>
       </c>
-      <c r="H22" t="n">
-        <v>271.2</v>
-      </c>
-      <c r="I22" t="inlineStr">
-        <is>
-          <t>арестованное, наличие ограничений: запрет на регистрационные действия</t>
-        </is>
-      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>21:10:200110:159</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr"/>
       <c r="J22" t="inlineStr">
         <is>
-          <t>арестованное, наличие ограничений: запрет на регистрационные действия</t>
+          <t>EA</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t xml:space="preserve">здание нежилое </t>
-        </is>
-      </c>
-      <c r="L22" t="inlineStr">
-        <is>
-          <t>21:10:200110:159</t>
-        </is>
-      </c>
-      <c r="M22" t="inlineStr">
-        <is>
-          <t>21:10:200110:159</t>
-        </is>
-      </c>
-      <c r="N22" t="inlineStr"/>
-      <c r="O22" t="inlineStr"/>
-      <c r="P22" t="inlineStr"/>
+          <t>Должников</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -1743,17 +1487,15 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Должников</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>EA</t>
-        </is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>2.1</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>нежилое помещение, площадью 2,10 кв. м, расположенное по адресу: Чувашская Республика, г. Чебоксары, ул. Академика Королева д.4, пом.17, кадастровый № 21:01:010901:2400</t>
+          <t xml:space="preserve">нежилое помещение, площадью 2,10 кв. м, </t>
         </is>
       </c>
       <c r="F23" t="n">
@@ -1764,37 +1506,22 @@
           <t>08/07/22 17:00</t>
         </is>
       </c>
-      <c r="H23" t="n">
-        <v>2.1</v>
-      </c>
-      <c r="I23" t="inlineStr">
-        <is>
-          <t>арестованное, наличие ограничений: запрет на регистрационные действия</t>
-        </is>
-      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>21:01:010901:2400</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr"/>
       <c r="J23" t="inlineStr">
         <is>
-          <t>арестованное, наличие ограничений: запрет на регистрационные действия</t>
+          <t>EA</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>нежилое помещение</t>
-        </is>
-      </c>
-      <c r="L23" t="inlineStr">
-        <is>
-          <t>21:01:010901:2400</t>
-        </is>
-      </c>
-      <c r="M23" t="inlineStr">
-        <is>
-          <t>21:01:010901:2400</t>
-        </is>
-      </c>
-      <c r="N23" t="inlineStr"/>
-      <c r="O23" t="inlineStr"/>
-      <c r="P23" t="inlineStr"/>
+          <t>Должников</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -1807,17 +1534,15 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Должников</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>EA</t>
-        </is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>3.2</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>2/3 доли нежилого помещения площадью 3,2 кв.м., расположенное по адресу: Чувашская Республика, г. Чебоксары, ул. М. Павлова, д. 43, пом.26, кадастровый № 21:01:000000:27943</t>
+          <t xml:space="preserve">2/3 доли нежилого помещения площадью 3,2 кв.м., </t>
         </is>
       </c>
       <c r="F24" t="n">
@@ -1828,37 +1553,22 @@
           <t>08/07/22 17:00</t>
         </is>
       </c>
-      <c r="H24" t="n">
-        <v>3.2</v>
-      </c>
-      <c r="I24" t="inlineStr">
-        <is>
-          <t>арестованное, наличие ограничений: запрет на регистрационные действия</t>
-        </is>
-      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>21:01:000000:27943</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr"/>
       <c r="J24" t="inlineStr">
         <is>
-          <t xml:space="preserve"> арестованное, наличие ограничений: запрет на регистрационные действия</t>
+          <t>EA</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>Нежилое помещение</t>
-        </is>
-      </c>
-      <c r="L24" t="inlineStr">
-        <is>
-          <t>21:01:000000:27943</t>
-        </is>
-      </c>
-      <c r="M24" t="inlineStr">
-        <is>
-          <t>21:01:000000:27943</t>
-        </is>
-      </c>
-      <c r="N24" t="inlineStr"/>
-      <c r="O24" t="inlineStr"/>
-      <c r="P24" t="inlineStr"/>
+          <t>Должников</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -1871,17 +1581,15 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Муниципальное</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>EA</t>
-        </is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>237.4</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Нежилое помещение, назначение: нежилое, количество этажей - 1, площадь - 237,4 кв. м, инвентарный N Р19/450-3-н, расположенное по адресу: Чувашская Республика - Чувашия, р-н Урмарский, д. Саруй, ул. Молодежная, д. 2а, пом. 2, кадастровый номер 21:19:110301:628</t>
+          <t xml:space="preserve">Нежилое помещение, назначение: нежилое, количество этажей - 1, площадь - 237,4 кв. м, инвентарный N Р19/450-3-н, </t>
         </is>
       </c>
       <c r="F25" t="n">
@@ -1892,29 +1600,22 @@
           <t>17/07/22 17:00</t>
         </is>
       </c>
-      <c r="H25" t="n">
-        <v>237.4</v>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>21:19:110301:628</t>
+        </is>
       </c>
       <c r="I25" t="inlineStr"/>
-      <c r="J25" t="inlineStr"/>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>EA</t>
+        </is>
+      </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>нежилое помещение</t>
-        </is>
-      </c>
-      <c r="L25" t="inlineStr">
-        <is>
-          <t>21:19:110301:628</t>
-        </is>
-      </c>
-      <c r="M25" t="inlineStr"/>
-      <c r="N25" t="inlineStr"/>
-      <c r="O25" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="P25" t="inlineStr"/>
+          <t>Муниципальное</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -1927,17 +1628,15 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Муниципальное</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>EA</t>
-        </is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>473.7</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Нежилое помещение, помещение 2б, расположенное на первом этаже двухэтажного кир-пичного нежилого здания, площадь ОКС’а 117,20 кв.м., кадастровый №21:19:170103:2962,Нежилое помещение, помещение 2в, расположенное на первом и втором этажах двухэтажного кирпичного нежилого здания, площадь ОКС’а 77,20 кв.м., кадастровый №21:19:170103:2964,Нежилое помещение, помещение 2г, расположенное на втором этаже двухэтажного кирпичного нежилого здания, площадь ОКС’а 279,30 кв.м., кадастровый №21:19:170103:2963</t>
+          <t>Нежилое помещение, помещение 2б, расположенное на первом этаже двухэтажного кир-пичного нежилого здания, площадь ОКС’а 117,20 кв.м.,Нежилое помещение, помещение 2в, расположенное на первом и втором этажах двухэтажного кирпичного нежилого здания, площадь ОКС’а 77,20 кв.м.,Нежилое помещение, помещение 2г, расположенное на втором этаже двухэтажного кирпичного нежилого здания, площадь ОКС’а 279,30 кв.м.</t>
         </is>
       </c>
       <c r="F26" t="n">
@@ -1948,21 +1647,22 @@
           <t>17/07/22 17:00</t>
         </is>
       </c>
-      <c r="H26" t="n">
-        <v>473.7</v>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>21:19:170103:2962</t>
+        </is>
       </c>
       <c r="I26" t="inlineStr"/>
-      <c r="J26" t="inlineStr"/>
-      <c r="K26" t="inlineStr"/>
-      <c r="L26" t="inlineStr"/>
-      <c r="M26" t="inlineStr"/>
-      <c r="N26" t="inlineStr"/>
-      <c r="O26" t="inlineStr">
-        <is>
-          <t>1-2</t>
-        </is>
-      </c>
-      <c r="P26" t="inlineStr"/>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>EA</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>Муниципальное</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -1975,17 +1675,15 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Должников</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>EA</t>
-        </is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>20.2</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Нежилое помещение, площадью 20,20 кв. м, расположенное по адресу: Чувашская Республика, г. Новочебоксарск, гаражный кооператив № 7 "Прогресс", гараж-бокс № 665, кадастровый номер 21:02:010905:1073</t>
+          <t xml:space="preserve">Нежилое помещение, площадью 20,20 кв. м, </t>
         </is>
       </c>
       <c r="F27" t="n">
@@ -1996,25 +1694,22 @@
           <t>13/07/22 14:00</t>
         </is>
       </c>
-      <c r="H27" t="n">
-        <v>20.2</v>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>21:02:010905:1073</t>
+        </is>
       </c>
       <c r="I27" t="inlineStr"/>
-      <c r="J27" t="inlineStr"/>
-      <c r="K27" t="inlineStr"/>
-      <c r="L27" t="inlineStr">
-        <is>
-          <t>21:02:010905:1073</t>
-        </is>
-      </c>
-      <c r="M27" t="inlineStr">
-        <is>
-          <t>21:02:010905:1073</t>
-        </is>
-      </c>
-      <c r="N27" t="inlineStr"/>
-      <c r="O27" t="inlineStr"/>
-      <c r="P27" t="inlineStr"/>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>EA</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>Должников</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -2027,17 +1722,15 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Должников</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>EA</t>
-        </is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>2.5</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>1/2 доля в праве общей долевой собственности на нежилое помещение (кладовая), площадью 2,50 кв. м, расположенное по адресу: Чувашская Республика, г. Чебоксары, проспект Тракторостроителей, д. 34, корпус 1, хозяйственная кладовая № 19, кадастровый номер 21:01:030407:7173</t>
+          <t xml:space="preserve">1/2 доля в праве общей долевой собственности на нежилое помещение (кладовая), площадью 2,50 кв. м, </t>
         </is>
       </c>
       <c r="F28" t="n">
@@ -2048,25 +1741,22 @@
           <t>13/07/22 14:00</t>
         </is>
       </c>
-      <c r="H28" t="n">
-        <v>2.5</v>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>21:01:030407:7173</t>
+        </is>
       </c>
       <c r="I28" t="inlineStr"/>
-      <c r="J28" t="inlineStr"/>
-      <c r="K28" t="inlineStr"/>
-      <c r="L28" t="inlineStr">
-        <is>
-          <t>21:01:030407:7173</t>
-        </is>
-      </c>
-      <c r="M28" t="inlineStr">
-        <is>
-          <t>21:01:030407:7173</t>
-        </is>
-      </c>
-      <c r="N28" t="inlineStr"/>
-      <c r="O28" t="inlineStr"/>
-      <c r="P28" t="inlineStr"/>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>EA</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>Должников</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -2079,17 +1769,15 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Муниципальное</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>PP</t>
-        </is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>31.2</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Муниципальное имущество города Шумерля Чувашской Республики: нежилое помещение в многоквартирном доме общей площадью 31,2 кв.м, кадастровый номер: 21:05:010119:220, расположенное по адресу: Чувашская Республика, город Шумерля, улица Карла Маркса, дом 21.</t>
+          <t xml:space="preserve">Муниципальное имущество города Шумерля Чувашской Республики: нежилое помещение в многоквартирном доме общей площадью 31,2 кв.м, </t>
         </is>
       </c>
       <c r="F29" t="n">
@@ -2100,35 +1788,24 @@
           <t>25/07/22 13:00</t>
         </is>
       </c>
-      <c r="H29" t="n">
-        <v>31.2</v>
-      </c>
-      <c r="I29" t="inlineStr"/>
-      <c r="J29" t="inlineStr"/>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>21:05:010119:220</t>
+        </is>
+      </c>
+      <c r="I29" t="n">
+        <v>262418.83</v>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>PP</t>
+        </is>
+      </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>Нежилое</t>
-        </is>
-      </c>
-      <c r="L29" t="inlineStr">
-        <is>
-          <t>21:05:010239:1677</t>
-        </is>
-      </c>
-      <c r="M29" t="inlineStr">
-        <is>
-          <t>21:05:010119:220</t>
-        </is>
-      </c>
-      <c r="N29" t="n">
-        <v>262418.83</v>
-      </c>
-      <c r="O29" t="inlineStr">
-        <is>
-          <t>1 этаж в МКД</t>
-        </is>
-      </c>
-      <c r="P29" t="inlineStr"/>
+          <t>Муниципальное</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
get addr and get coord from dadata sugest(free)
</commit_message>
<xml_diff>
--- a/torgi/output.xlsx
+++ b/torgi/output.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="173">
   <si>
     <t>Регион</t>
   </si>
@@ -55,55 +55,301 @@
     <t>Имущество</t>
   </si>
   <si>
+    <t>Координаты</t>
+  </si>
+  <si>
+    <t>Коммерческая оценка.supermarket</t>
+  </si>
+  <si>
+    <t>Коммерческая оценка.convenience</t>
+  </si>
+  <si>
+    <t>Коммерческая оценка.dentist</t>
+  </si>
+  <si>
+    <t>Коммерческая оценка.mobile_phone</t>
+  </si>
+  <si>
+    <t>Коммерческая оценка.jewelry</t>
+  </si>
+  <si>
+    <t>Коммерческая оценка.residents</t>
+  </si>
+  <si>
+    <t>Коммерческая оценка.bus_stop</t>
+  </si>
+  <si>
+    <t>Коммерческая оценка.fire_station</t>
+  </si>
+  <si>
+    <t>Коммерческая оценка.chemist</t>
+  </si>
+  <si>
+    <t>Коммерческая оценка.alcohol</t>
+  </si>
+  <si>
+    <t>Коммерческая оценка.parking</t>
+  </si>
+  <si>
+    <t>Коммерческая оценка.playground</t>
+  </si>
+  <si>
+    <t>Коммерческая оценка.school</t>
+  </si>
+  <si>
+    <t>Коммерческая оценка.public_bath</t>
+  </si>
+  <si>
+    <t>Коммерческая оценка.fishing</t>
+  </si>
+  <si>
+    <t>Коммерческая оценка.pharmacy</t>
+  </si>
+  <si>
+    <t>Коммерческая оценка.kindergarten</t>
+  </si>
+  <si>
+    <t>Коммерческая оценка.fuel</t>
+  </si>
+  <si>
+    <t>Коммерческая оценка.cafe</t>
+  </si>
+  <si>
+    <t>Коммерческая оценка.furniture</t>
+  </si>
+  <si>
+    <t>Коммерческая оценка.doityourself</t>
+  </si>
+  <si>
+    <t>Коммерческая оценка</t>
+  </si>
+  <si>
+    <t>Коммерческая оценка.bar</t>
+  </si>
+  <si>
+    <t>Коммерческая оценка.seafood</t>
+  </si>
+  <si>
+    <t>Коммерческая оценка.clothes</t>
+  </si>
+  <si>
+    <t>Коммерческая оценка.craft</t>
+  </si>
+  <si>
+    <t>Коммерческая оценка.bakery</t>
+  </si>
+  <si>
+    <t>Коммерческая оценка.veterinary</t>
+  </si>
+  <si>
+    <t>Коммерческая оценка.car_parts</t>
+  </si>
+  <si>
+    <t>Коммерческая оценка.beauty</t>
+  </si>
+  <si>
+    <t>Коммерческая оценка.pub</t>
+  </si>
+  <si>
+    <t>Коммерческая оценка.sports_centre</t>
+  </si>
+  <si>
+    <t>Коммерческая оценка.courthouse</t>
+  </si>
+  <si>
+    <t>Коммерческая оценка.police</t>
+  </si>
+  <si>
+    <t>Коммерческая оценка.service</t>
+  </si>
+  <si>
+    <t>Коммерческая оценка.car_repair</t>
+  </si>
+  <si>
+    <t>Коммерческая оценка.bank</t>
+  </si>
+  <si>
+    <t>Коммерческая оценка.recycling</t>
+  </si>
+  <si>
+    <t>Коммерческая оценка.paint</t>
+  </si>
+  <si>
+    <t>Коммерческая оценка.kiosk</t>
+  </si>
+  <si>
+    <t>Коммерческая оценка.atm</t>
+  </si>
+  <si>
+    <t>Коммерческая оценка.post_office</t>
+  </si>
+  <si>
+    <t>Коммерческая оценка.fast_food</t>
+  </si>
+  <si>
+    <t>Коммерческая оценка.lighting</t>
+  </si>
+  <si>
+    <t>Коммерческая оценка.car_wash</t>
+  </si>
+  <si>
+    <t>Коммерческая оценка.drinking_water</t>
+  </si>
+  <si>
+    <t>Коммерческая оценка.tattoo</t>
+  </si>
+  <si>
+    <t>Коммерческая оценка.clinic</t>
+  </si>
+  <si>
+    <t>Коммерческая оценка.photo_studio</t>
+  </si>
+  <si>
+    <t>Коммерческая оценка.shoes</t>
+  </si>
+  <si>
+    <t>Коммерческая оценка.restaurant</t>
+  </si>
+  <si>
+    <t>Коммерческая оценка.confectionery</t>
+  </si>
+  <si>
+    <t>Коммерческая оценка.driving_school</t>
+  </si>
+  <si>
+    <t>Коммерческая оценка.department_store</t>
+  </si>
+  <si>
+    <t>Коммерческая оценка.florist</t>
+  </si>
+  <si>
+    <t>Коммерческая оценка.curtain</t>
+  </si>
+  <si>
+    <t>Коммерческая оценка.dry_cleaning</t>
+  </si>
+  <si>
     <t>21</t>
   </si>
   <si>
+    <t>12</t>
+  </si>
+  <si>
     <t>58</t>
   </si>
   <si>
+    <t>16</t>
+  </si>
+  <si>
     <t>91</t>
   </si>
   <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>12</t>
+    <t>Нежилое помещение.</t>
+  </si>
+  <si>
+    <t>Нежилое помещение .</t>
+  </si>
+  <si>
+    <t>Помещение</t>
+  </si>
+  <si>
+    <t>Помещение 1002, нежилое, Этаж № 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Помещение, назначение – нежилое., количество этажей – 1, 2по </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Помещение, назначение – нежилое., количество этажей - 1по </t>
+  </si>
+  <si>
+    <t>Нежилое помещение, общ., этаж 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Цех по производству стального литья, 1-й пусковой  корпус S= 10523,1 кв.мстоимость 62 185 149,66 руб. (вкл. НДС 20%). Земельный участокстоимость 34 472 600,0 руб. </t>
   </si>
   <si>
     <t>Нежилое помещение</t>
   </si>
   <si>
-    <t xml:space="preserve">Нежилое помещение </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Муниципальное имущество города Шумерля Чувашской Республики: нежилое помещение в многоквартирном доме </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Помещение , назначение: нежилое; наименование: нежилое помещение; номер, тип этажа, на котором расположено помещение: этаж № 2; </t>
-  </si>
-  <si>
-    <t>Нежилое помещение, помещение 2б, расположенное на первом этаже двухэтажного кир-пичного нежилого здания.Нежилое помещение, помещение 2в, расположенное на первом и втором этажах двухэтажного кирпичного нежилого здания.Нежилое помещение, помещение 2г, расположенное на втором этаже двухэтажного кирпичного нежилого здания.</t>
-  </si>
-  <si>
-    <t>Нежилое помещение, назначение: нежилое, количество этажей - 1, инвентарный N Р19/450-3-н</t>
-  </si>
-  <si>
-    <t xml:space="preserve">помещения 1 этажа и подвала </t>
-  </si>
-  <si>
-    <t xml:space="preserve">помещения 1 этажа </t>
-  </si>
-  <si>
-    <t xml:space="preserve">помещения 2 этажа </t>
-  </si>
-  <si>
-    <t>Помещение, назначение: нежилое, этаж 1, номера на поэтажном плане поз. 1 - 13, 15 - 22</t>
-  </si>
-  <si>
-    <t>Нежилое помещение .с земельным участком (для размещения хозяйственного магазина) .</t>
-  </si>
-  <si>
-    <t>Нежилое помещение .</t>
+    <t>нежилое помещение</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Земельный уч-к </t>
+  </si>
+  <si>
+    <t>Нежилые помещения № 1,2,3,4,5, расположенные на 2-м этаже,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">помещение , назначение: нежилое; наименование: нежилое помещение; номер, тип этажа, на котором расположено помещение: этаж № 1; </t>
+  </si>
+  <si>
+    <t>Помещение, назначение: нежилое, этажей: 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Нежилое здание (Уборная), </t>
+  </si>
+  <si>
+    <t>Нежилое  помещение.</t>
+  </si>
+  <si>
+    <t>Чувашская Республика - Чувашия, г Козловка, ул Маяковского, д 6А, помещ 1</t>
+  </si>
+  <si>
+    <t>г Йошкар-Ола, ул Машиностроителей, д 107А, помещ 1-13</t>
+  </si>
+  <si>
+    <t>Пензенская обл, Бессоновский р-н, с Кижеватово, ул Молодежная, д 28, кв 7</t>
+  </si>
+  <si>
+    <t>Респ Марий Эл, пгт Морки, ул Мира, д 42, помещ 5</t>
+  </si>
+  <si>
+    <t>Республика Марий Эл, Моркинский район, пгт. Морки, ул. Мира, д.42, пом. 2 (поз. 25-30)</t>
+  </si>
+  <si>
+    <t>Пензенская обл, г Заречный, ул Зеленая, д 10Д, помещ 40</t>
+  </si>
+  <si>
+    <t>Респ Татарстан, г Набережные Челны, ул Профильная, д 59</t>
+  </si>
+  <si>
+    <t>г Чебоксары, ул Болгарстроя, д 5, помещ 11</t>
+  </si>
+  <si>
+    <t>г Чебоксары, ул Болгарстроя, д 5, помещ 8</t>
+  </si>
+  <si>
+    <t>Чувашская Республика, г. Чебоксары, ул. Ленинского Комсомола, д. 23, корпус 1, кладовая №9</t>
+  </si>
+  <si>
+    <t>г Чебоксары, ул Болгарстроя, д 5, помещ 10</t>
+  </si>
+  <si>
+    <t>Чувашская Республика - Чувашия, г Новочебоксарск, ул Промышленная, влд 78</t>
+  </si>
+  <si>
+    <t>г Чебоксары, ул Сельская, д 39, помещ 45</t>
+  </si>
+  <si>
+    <t>Республика Татарстан, Заинский муниципальный район, Сармаш-Башское сельское поселение, с. Федоровка, ул. Клубная, д.27а, кв. 1Н .</t>
+  </si>
+  <si>
+    <t>установлено относительно ориентира, расположенного в границах участка. Почтовый адрес ориентира: Пензенская область, р-н Колышлейский, с. Колтовское, ул. Боевая, д. 26А., Нежилое помещение адрес: Пензенская область, Колышлейский район, с.Колтовское, ул.Боевая, 26А, Нежилое помещение адрес: Пензенская область, Колышлейский район, с.Колтовское, ул.Боевая, 26А, Нежилое здание адрес: Пензенская область, р-н. Колышлейский, с. Колтовское, ул. Боевая, д. 27</t>
+  </si>
+  <si>
+    <t>422230, РТ, г. Агрыз, ул. К. Маркса, д.74, расположенные по адресу РТ, г.Агрыз, ул.К.Маркса, д.74</t>
+  </si>
+  <si>
+    <t>Пензенская область, г Пенза, ул. Пушанина, д. 6; .</t>
+  </si>
+  <si>
+    <t>Чувашская Республика, г. Новочебоксарск, ул. Южная, д. 6, пом. 165</t>
+  </si>
+  <si>
+    <t>Республика Крым, р-н Симферопольский, с Перово, ул Таврическая.Площадь 28,9 . Коммуникации и инженерное обеспечение: отсутствуют..</t>
+  </si>
+  <si>
+    <t>расположения: Россия,  Чувашская Республика, Канашский район, д. Новое Урюмово, ул. Кооперативная, д.31 е, пом. 1</t>
   </si>
   <si>
     <t>Чувашская Республика, г. Чебоксары, ул. Ленинского Комсомола, д. 25, корп. 1, пом. 10.4</t>
@@ -124,67 +370,112 @@
     <t>Чувашская Республика, Чебоксарский район, Синьяльское сельское поселение, д. Аркасы, ул. Садовая, д. 35 А, пом. 7</t>
   </si>
   <si>
-    <t>г. Пенза, ул. Ново - Тамбовская, 29</t>
-  </si>
-  <si>
-    <t>Чувашская Республика, город Шумерля, улица Карла Маркса, дом 21.</t>
-  </si>
-  <si>
-    <t>Пензенская область, г. Пенза, Октябрьский район, Пятый Виноградный проезд, д. 18; .</t>
-  </si>
-  <si>
-    <t>Чувашская Республика - Чувашия, р-н Урмарский, д. Саруй, ул. Молодежная, д. 2а, пом. 2</t>
-  </si>
-  <si>
-    <t>по ул.Габдуллы Тукая, д.92, пом.1001</t>
-  </si>
-  <si>
-    <t>по ул.Центральная, д.40а, кв.1001, (ж.м.Отары)</t>
-  </si>
-  <si>
-    <t>по ул.Габдуллы Тукая, д.92, пом.1000</t>
-  </si>
-  <si>
-    <t>по ул.Центральная, д.40а, кв.1002, (ж.м.Отары)</t>
-  </si>
-  <si>
-    <t>по ул.Центральная, д.40а, пом.1003, (ж.м.Отары)</t>
-  </si>
-  <si>
-    <t>Республика Марий Эл, г. Йошкар-Ола, ул. Красноармейская, д. 103а</t>
-  </si>
-  <si>
-    <t>РМЭ, Медведевский район, с. Азаново, ул. Советская, д.13А, принадлежащие ПК «Медведевское райпо»</t>
-  </si>
-  <si>
-    <t>РМЭ, Медведевский район, п. Сурок, ул. Мира, д.4, принадлежащее ПК «Медведевское райпо».</t>
+    <t>29 08 22 14:00</t>
+  </si>
+  <si>
+    <t>25 08 22 21:00</t>
+  </si>
+  <si>
+    <t>24 08 22 14:00</t>
+  </si>
+  <si>
+    <t>27 08 22 05:00</t>
+  </si>
+  <si>
+    <t>23 08 22 14:00</t>
+  </si>
+  <si>
+    <t>08 08 22 14:00</t>
+  </si>
+  <si>
+    <t>19 08 22 09:00</t>
+  </si>
+  <si>
+    <t>15 08 22 14:00</t>
+  </si>
+  <si>
+    <t>22 08 22 14:00</t>
+  </si>
+  <si>
+    <t>17 08 22 14:00</t>
+  </si>
+  <si>
+    <t>14 08 22 05:00</t>
+  </si>
+  <si>
+    <t>12 08 22 20:00</t>
+  </si>
+  <si>
+    <t>11 08 22 20:59</t>
+  </si>
+  <si>
+    <t>09 08 22 05:00</t>
   </si>
   <si>
     <t>01 08 22 14:00</t>
   </si>
   <si>
-    <t>01 08 22 06:00</t>
-  </si>
-  <si>
-    <t>26 07 22 13:00</t>
-  </si>
-  <si>
-    <t>25 07 22 13:00</t>
-  </si>
-  <si>
-    <t>18 07 22 20:00</t>
-  </si>
-  <si>
-    <t>17 07 22 17:00</t>
-  </si>
-  <si>
-    <t>12 07 22 09:00</t>
-  </si>
-  <si>
-    <t>11 07 22 14:30</t>
-  </si>
-  <si>
-    <t>11 07 22 14:00</t>
+    <t xml:space="preserve">21:12:000000:7595 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">12:05:0301005:413, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">58:05:0160203:870, </t>
+  </si>
+  <si>
+    <t>16:05:010504:438</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12:13:0990117:580, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">12:13:0990117:577, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">58:34:0010141:710, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">16:52:080201:142, </t>
+  </si>
+  <si>
+    <t>21:01:030702:1810</t>
+  </si>
+  <si>
+    <t>21:01:030702:1809</t>
+  </si>
+  <si>
+    <t>21:01:030310:4184</t>
+  </si>
+  <si>
+    <t>21:01:030702:1806</t>
+  </si>
+  <si>
+    <t>21:02:000000:32513</t>
+  </si>
+  <si>
+    <t>21:02:000000:32517</t>
+  </si>
+  <si>
+    <t>21:01:010103:544</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16:19:090301:75 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">58:12:1901007:308, </t>
+  </si>
+  <si>
+    <t>16:01:110301:4410</t>
+  </si>
+  <si>
+    <t>58:29:3008002:4765</t>
+  </si>
+  <si>
+    <t>90:12:130101:188</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21:11:290501:799, </t>
   </si>
   <si>
     <t>21:01:030310:2531</t>
@@ -205,52 +496,46 @@
     <t>21:02:010510:988</t>
   </si>
   <si>
-    <t xml:space="preserve">21:05:010119:220, </t>
-  </si>
-  <si>
-    <t>58:29:1007005:5650</t>
-  </si>
-  <si>
-    <t>21:19:170103:2962,</t>
-  </si>
-  <si>
-    <t>21:19:110301:628</t>
-  </si>
-  <si>
-    <t>16:50:011716:479</t>
-  </si>
-  <si>
-    <t>16:50:170532:88</t>
-  </si>
-  <si>
-    <t>16:50:011716:165</t>
-  </si>
-  <si>
-    <t>16:50:170532:89</t>
-  </si>
-  <si>
-    <t>16:50:170532:90</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12:05:0000000:12935, </t>
-  </si>
-  <si>
-    <t xml:space="preserve">12:04:0270104:71 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">12:04:0261801:11, </t>
-  </si>
-  <si>
     <t>EA</t>
   </si>
   <si>
-    <t>PP</t>
+    <t>BOC</t>
+  </si>
+  <si>
+    <t>Муниципальное</t>
   </si>
   <si>
     <t>Должников</t>
   </si>
   <si>
-    <t>Муниципальное</t>
+    <t>55.8381033, 48.2433137</t>
+  </si>
+  <si>
+    <t>56.625846, 47.839987</t>
+  </si>
+  <si>
+    <t>53.2089787, 45.3058647</t>
+  </si>
+  <si>
+    <t>None, None</t>
+  </si>
+  <si>
+    <t>56.4371736, 49.0194425</t>
+  </si>
+  <si>
+    <t>53.187823, 45.174578</t>
+  </si>
+  <si>
+    <t>55.652554, 52.2976953</t>
+  </si>
+  <si>
+    <t>56.0709455, 47.2817658</t>
+  </si>
+  <si>
+    <t>56.0790839, 47.5070169</t>
+  </si>
+  <si>
+    <t>56.15064, 47.183184</t>
   </si>
 </sst>
 </file>
@@ -634,7 +919,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M21"/>
+  <dimension ref="A1:BS29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -651,7 +936,7 @@
     <col min="11" max="11" width="12.7109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:71">
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
@@ -688,776 +973,1718 @@
       <c r="M1" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:13">
+      <c r="N1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="X1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="AG1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="AJ1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="AK1" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="AL1" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="AM1" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="AN1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="AO1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="AP1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="AQ1" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="AR1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="AS1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="AT1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="AU1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="AV1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="AW1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="AX1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="AY1" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="AZ1" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="BA1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="BB1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="BC1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="BD1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="BE1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="BF1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="BG1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="BH1" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="BI1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="BJ1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="BK1" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="BL1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="BM1" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="BN1" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="BO1" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="BP1" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="BQ1" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="BR1" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="BS1" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:71">
       <c r="A2" s="4">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>70</v>
       </c>
       <c r="C2" s="1">
-        <v>186</v>
+        <v>33</v>
       </c>
       <c r="D2" s="2">
-        <f>HYPERLINK("https://torgi.gov.ru/new/public/lots/lot/21000025550000000040_8/(lotInfo:info)", "21000025550000000040_8")</f>
+        <f>HYPERLINK("https://torgi.gov.ru/new/public/lots/lot/22000018250000000008_1/(lotInfo:info)", "22000018250000000008_1")</f>
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>75</v>
       </c>
       <c r="F2" s="3">
-        <v>44708.77956989247</v>
+        <v>11358</v>
       </c>
       <c r="G2" s="3">
-        <v>8315833</v>
+        <v>374814</v>
       </c>
       <c r="H2" t="s">
-        <v>29</v>
+        <v>91</v>
       </c>
       <c r="I2" t="s">
-        <v>47</v>
+        <v>117</v>
       </c>
       <c r="J2" t="s">
-        <v>56</v>
+        <v>132</v>
       </c>
       <c r="L2" t="s">
-        <v>74</v>
+        <v>159</v>
       </c>
       <c r="M2" t="s">
+        <v>161</v>
+      </c>
+      <c r="N2" t="s">
+        <v>163</v>
+      </c>
+      <c r="O2">
+        <v>2</v>
+      </c>
+      <c r="P2">
+        <v>8</v>
+      </c>
+      <c r="Q2">
+        <v>1</v>
+      </c>
+      <c r="R2">
+        <v>1</v>
+      </c>
+      <c r="S2">
+        <v>1</v>
+      </c>
+      <c r="T2">
+        <v>3531</v>
+      </c>
+      <c r="U2">
+        <v>1</v>
+      </c>
+      <c r="V2">
+        <v>1</v>
+      </c>
+      <c r="W2">
+        <v>1</v>
+      </c>
+      <c r="X2">
+        <v>2</v>
+      </c>
+      <c r="Y2">
+        <v>2</v>
+      </c>
+      <c r="Z2">
+        <v>1</v>
+      </c>
+      <c r="AA2">
+        <v>1</v>
+      </c>
+      <c r="AB2">
+        <v>1</v>
+      </c>
+      <c r="AC2">
+        <v>2</v>
+      </c>
+      <c r="AD2">
+        <v>1</v>
+      </c>
+      <c r="AE2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:71">
+      <c r="A3" s="4">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" s="1">
+        <v>644.1</v>
+      </c>
+      <c r="D3" s="2">
+        <f>HYPERLINK("https://torgi.gov.ru/new/public/lots/lot/21000025550000000052_1/(lotInfo:info)", "21000025550000000052_1")</f>
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="3" spans="1:13">
-      <c r="A3" s="4">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="1">
-        <v>154.6</v>
-      </c>
-      <c r="D3" s="2">
-        <f>HYPERLINK("https://torgi.gov.ru/new/public/lots/lot/21000025550000000040_6/(lotInfo:info)", "21000025550000000040_6")</f>
-        <v>0</v>
-      </c>
-      <c r="E3" t="s">
-        <v>17</v>
-      </c>
       <c r="F3" s="3">
-        <v>37106.51358344114</v>
+        <v>18431.40350877193</v>
       </c>
       <c r="G3" s="3">
-        <v>5736667</v>
+        <v>11871667</v>
       </c>
       <c r="H3" t="s">
-        <v>30</v>
+        <v>92</v>
       </c>
       <c r="I3" t="s">
-        <v>47</v>
+        <v>118</v>
       </c>
       <c r="J3" t="s">
-        <v>57</v>
+        <v>133</v>
       </c>
       <c r="L3" t="s">
-        <v>74</v>
+        <v>159</v>
       </c>
       <c r="M3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
+        <v>162</v>
+      </c>
+      <c r="N3" t="s">
+        <v>164</v>
+      </c>
+      <c r="T3">
+        <v>254</v>
+      </c>
+      <c r="U3">
+        <v>2</v>
+      </c>
+      <c r="AF3">
+        <v>1</v>
+      </c>
+      <c r="AG3">
+        <v>1</v>
+      </c>
+      <c r="AH3">
+        <v>1</v>
+      </c>
+      <c r="AI3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:71">
       <c r="A4" s="4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>72</v>
       </c>
       <c r="C4" s="1">
-        <v>194</v>
+        <v>60.4</v>
       </c>
       <c r="D4" s="2">
-        <f>HYPERLINK("https://torgi.gov.ru/new/public/lots/lot/21000025550000000040_5/(lotInfo:info)", "21000025550000000040_5")</f>
+        <f>HYPERLINK("https://torgi.gov.ru/new/public/lots/lot/21000025550000000050_11/(lotInfo:info)", "21000025550000000050_11")</f>
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>77</v>
       </c>
       <c r="F4" s="3">
-        <v>44707.90206185567</v>
+        <v>21688.74172185431</v>
       </c>
       <c r="G4" s="3">
-        <v>8673333</v>
+        <v>1310000</v>
       </c>
       <c r="H4" t="s">
-        <v>31</v>
+        <v>93</v>
       </c>
       <c r="I4" t="s">
-        <v>47</v>
+        <v>119</v>
       </c>
       <c r="J4" t="s">
-        <v>58</v>
+        <v>134</v>
       </c>
       <c r="L4" t="s">
-        <v>74</v>
+        <v>159</v>
       </c>
       <c r="M4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13">
+        <v>162</v>
+      </c>
+      <c r="N4" t="s">
+        <v>165</v>
+      </c>
+      <c r="P4">
+        <v>3</v>
+      </c>
+      <c r="T4">
+        <v>1533</v>
+      </c>
+    </row>
+    <row r="5" spans="1:71">
       <c r="A5" s="4">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>73</v>
       </c>
       <c r="C5" s="1">
-        <v>143.6</v>
+        <v>26.9</v>
       </c>
       <c r="D5" s="2">
-        <f>HYPERLINK("https://torgi.gov.ru/new/public/lots/lot/21000025550000000040_7/(lotInfo:info)", "21000025550000000040_7")</f>
+        <f>HYPERLINK("https://torgi.gov.ru/new/public/lots/lot/21000029570000000011_1/(lotInfo:info)", "21000029570000000011_1")</f>
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>78</v>
       </c>
       <c r="F5" s="3">
-        <v>37523.21030640668</v>
+        <v>21521.00371747212</v>
       </c>
       <c r="G5" s="3">
-        <v>5388333</v>
-      </c>
-      <c r="H5" t="s">
-        <v>32</v>
+        <v>578915</v>
       </c>
       <c r="I5" t="s">
-        <v>47</v>
+        <v>120</v>
       </c>
       <c r="J5" t="s">
-        <v>59</v>
+        <v>135</v>
+      </c>
+      <c r="K5" s="3">
+        <v>668951.35</v>
       </c>
       <c r="L5" t="s">
-        <v>74</v>
+        <v>159</v>
       </c>
       <c r="M5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13">
+        <v>161</v>
+      </c>
+      <c r="N5" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="6" spans="1:71">
       <c r="A6" s="4">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>71</v>
       </c>
       <c r="C6" s="1">
-        <v>126.2</v>
+        <v>476.6</v>
       </c>
       <c r="D6" s="2">
-        <f>HYPERLINK("https://torgi.gov.ru/new/public/lots/lot/21000025550000000040_9/(lotInfo:info)", "21000025550000000040_9")</f>
+        <f>HYPERLINK("https://torgi.gov.ru/new/public/lots/lot/21000022630000000002_10/(lotInfo:info)", "21000022630000000002_10")</f>
         <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>17</v>
+        <v>79</v>
       </c>
       <c r="F6" s="3">
-        <v>37731.11727416798</v>
+        <v>2248.006714225766</v>
       </c>
       <c r="G6" s="3">
-        <v>4761667</v>
+        <v>1071400</v>
       </c>
       <c r="H6" t="s">
-        <v>33</v>
+        <v>94</v>
       </c>
       <c r="I6" t="s">
-        <v>47</v>
+        <v>121</v>
       </c>
       <c r="J6" t="s">
-        <v>60</v>
+        <v>136</v>
       </c>
       <c r="L6" t="s">
-        <v>74</v>
+        <v>159</v>
       </c>
       <c r="M6" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13">
+        <v>161</v>
+      </c>
+      <c r="N6" t="s">
+        <v>167</v>
+      </c>
+      <c r="P6">
+        <v>1</v>
+      </c>
+      <c r="T6">
+        <v>2379</v>
+      </c>
+      <c r="AA6">
+        <v>1</v>
+      </c>
+      <c r="AE6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:71">
       <c r="A7" s="4">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>71</v>
       </c>
       <c r="C7" s="1">
-        <v>22.9</v>
+        <v>120.2</v>
       </c>
       <c r="D7" s="2">
-        <f>HYPERLINK("https://torgi.gov.ru/new/public/lots/lot/21000025550000000040_17/(lotInfo:info)", "21000025550000000040_17")</f>
+        <f>HYPERLINK("https://torgi.gov.ru/new/public/lots/lot/21000022630000000002_9/(lotInfo:info)", "21000022630000000002_9")</f>
         <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>17</v>
+        <v>80</v>
       </c>
       <c r="F7" s="3">
-        <v>10516.7248908297</v>
+        <v>3219.966722129784</v>
       </c>
       <c r="G7" s="3">
-        <v>240833</v>
+        <v>387040</v>
       </c>
       <c r="H7" t="s">
-        <v>34</v>
+        <v>95</v>
       </c>
       <c r="I7" t="s">
-        <v>47</v>
+        <v>121</v>
       </c>
       <c r="J7" t="s">
-        <v>61</v>
+        <v>137</v>
       </c>
       <c r="L7" t="s">
-        <v>74</v>
+        <v>159</v>
       </c>
       <c r="M7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13">
+        <v>161</v>
+      </c>
+      <c r="N7" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="8" spans="1:71">
       <c r="A8" s="4">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>72</v>
       </c>
       <c r="C8" s="1">
-        <v>1476.7</v>
+        <v>58.6</v>
       </c>
       <c r="D8" s="2">
-        <f>HYPERLINK("https://torgi.gov.ru/new/public/lots/lot/22000123100000000001_1/(lotInfo:info)", "22000123100000000001_1")</f>
-        <v>0</v>
+        <f>HYPERLINK("https://torgi.gov.ru/new/public/lots/lot/21000025550000000049_8/(lotInfo:info)", "21000025550000000049_8")</f>
+        <v>0</v>
+      </c>
+      <c r="E8" t="s">
+        <v>81</v>
       </c>
       <c r="F8" s="3">
-        <v>9683.754317058305</v>
+        <v>52849.82935153584</v>
       </c>
       <c r="G8" s="3">
-        <v>14300000</v>
+        <v>3097000</v>
       </c>
       <c r="H8" t="s">
-        <v>35</v>
+        <v>96</v>
       </c>
       <c r="I8" t="s">
-        <v>48</v>
+        <v>122</v>
+      </c>
+      <c r="J8" t="s">
+        <v>138</v>
       </c>
       <c r="L8" t="s">
-        <v>74</v>
+        <v>159</v>
       </c>
       <c r="M8" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13">
+        <v>162</v>
+      </c>
+      <c r="N8" t="s">
+        <v>168</v>
+      </c>
+      <c r="O8">
+        <v>3</v>
+      </c>
+      <c r="P8">
+        <v>1</v>
+      </c>
+      <c r="T8">
+        <v>7651</v>
+      </c>
+      <c r="U8">
+        <v>6</v>
+      </c>
+      <c r="X8">
+        <v>4</v>
+      </c>
+      <c r="AA8">
+        <v>1</v>
+      </c>
+      <c r="AD8">
+        <v>1</v>
+      </c>
+      <c r="AG8">
+        <v>1</v>
+      </c>
+      <c r="AK8">
+        <v>1</v>
+      </c>
+      <c r="AL8">
+        <v>1</v>
+      </c>
+      <c r="AM8">
+        <v>2</v>
+      </c>
+      <c r="AN8">
+        <v>1</v>
+      </c>
+      <c r="AO8">
+        <v>1</v>
+      </c>
+      <c r="AP8">
+        <v>1</v>
+      </c>
+      <c r="AQ8">
+        <v>2</v>
+      </c>
+      <c r="AR8">
+        <v>3</v>
+      </c>
+      <c r="AS8">
+        <v>1</v>
+      </c>
+      <c r="AT8">
+        <v>2</v>
+      </c>
+      <c r="AU8">
+        <v>1</v>
+      </c>
+      <c r="AV8">
+        <v>1</v>
+      </c>
+      <c r="AW8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:71">
       <c r="A9" s="4">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>73</v>
       </c>
       <c r="C9" s="1">
-        <v>478.7</v>
+        <v>21826</v>
       </c>
       <c r="D9" s="2">
-        <f>HYPERLINK("https://torgi.gov.ru/new/public/lots/lot/22000027070000000001_1/(lotInfo:info)", "22000027070000000001_1")</f>
+        <f>HYPERLINK("https://torgi.gov.ru/new/public/lots/lot/22000124620000000002_1/(lotInfo:info)", "22000124620000000002_1")</f>
         <v>0</v>
       </c>
       <c r="E9" t="s">
-        <v>18</v>
+        <v>82</v>
       </c>
       <c r="F9" s="3">
-        <v>13019.00981825778</v>
+        <v>4428.559958764776</v>
       </c>
       <c r="G9" s="3">
-        <v>6232200</v>
+        <v>96657749.66</v>
+      </c>
+      <c r="H9" t="s">
+        <v>97</v>
       </c>
       <c r="I9" t="s">
-        <v>49</v>
+        <v>123</v>
+      </c>
+      <c r="J9" t="s">
+        <v>139</v>
       </c>
       <c r="L9" t="s">
-        <v>74</v>
+        <v>159</v>
       </c>
       <c r="M9" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13">
+        <v>162</v>
+      </c>
+      <c r="N9" t="s">
+        <v>169</v>
+      </c>
+      <c r="T9">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="10" spans="1:71">
       <c r="A10" s="4">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>70</v>
       </c>
       <c r="C10" s="1">
-        <v>31.2</v>
+        <v>11.9</v>
       </c>
       <c r="D10" s="2">
-        <f>HYPERLINK("https://torgi.gov.ru/new/public/lots/lot/22000012370000000016_1/(lotInfo:info)", "22000012370000000016_1")</f>
+        <f>HYPERLINK("https://torgi.gov.ru/new/public/lots/lot/21000025550000000047_5/(lotInfo:info)", "21000025550000000047_5")</f>
         <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>19</v>
+        <v>83</v>
       </c>
       <c r="F10" s="3">
-        <v>26514.00641025641</v>
+        <v>29691.8487394958</v>
       </c>
       <c r="G10" s="3">
-        <v>827237</v>
+        <v>353333</v>
       </c>
       <c r="H10" t="s">
-        <v>36</v>
+        <v>98</v>
       </c>
       <c r="I10" t="s">
-        <v>50</v>
+        <v>124</v>
       </c>
       <c r="J10" t="s">
-        <v>62</v>
-      </c>
-      <c r="K10" s="3">
-        <v>262418.83</v>
+        <v>140</v>
       </c>
       <c r="L10" t="s">
-        <v>75</v>
+        <v>159</v>
       </c>
       <c r="M10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13">
+        <v>162</v>
+      </c>
+      <c r="N10" t="s">
+        <v>170</v>
+      </c>
+      <c r="O10">
+        <v>2</v>
+      </c>
+      <c r="T10">
+        <v>795</v>
+      </c>
+      <c r="U10">
+        <v>3</v>
+      </c>
+      <c r="AD10">
+        <v>1</v>
+      </c>
+      <c r="AG10">
+        <v>1</v>
+      </c>
+      <c r="AW10">
+        <v>3</v>
+      </c>
+      <c r="AX10">
+        <v>1</v>
+      </c>
+      <c r="AY10">
+        <v>1</v>
+      </c>
+      <c r="AZ10">
+        <v>1</v>
+      </c>
+      <c r="BA10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:71">
       <c r="A11" s="4">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>70</v>
       </c>
       <c r="C11" s="1">
-        <v>397.8</v>
+        <v>14.2</v>
       </c>
       <c r="D11" s="2">
-        <f>HYPERLINK("https://torgi.gov.ru/new/public/lots/lot/21000016520000000003_1/(lotInfo:info)", "21000016520000000003_1")</f>
+        <f>HYPERLINK("https://torgi.gov.ru/new/public/lots/lot/21000025550000000047_4/(lotInfo:info)", "21000025550000000047_4")</f>
         <v>0</v>
       </c>
       <c r="E11" t="s">
-        <v>20</v>
+        <v>83</v>
       </c>
       <c r="F11" s="3">
-        <v>22536.04826546003</v>
+        <v>29694.85915492958</v>
       </c>
       <c r="G11" s="3">
-        <v>8964840</v>
+        <v>421667</v>
       </c>
       <c r="H11" t="s">
-        <v>37</v>
+        <v>99</v>
       </c>
       <c r="I11" t="s">
-        <v>51</v>
+        <v>124</v>
       </c>
       <c r="J11" t="s">
-        <v>63</v>
-      </c>
-      <c r="K11" s="3">
-        <v>5481314.05</v>
+        <v>141</v>
       </c>
       <c r="L11" t="s">
-        <v>74</v>
+        <v>159</v>
       </c>
       <c r="M11" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13">
+        <v>162</v>
+      </c>
+      <c r="N11" t="s">
+        <v>170</v>
+      </c>
+      <c r="O11">
+        <v>2</v>
+      </c>
+      <c r="T11">
+        <v>795</v>
+      </c>
+      <c r="U11">
+        <v>3</v>
+      </c>
+      <c r="AD11">
+        <v>1</v>
+      </c>
+      <c r="AG11">
+        <v>1</v>
+      </c>
+      <c r="AW11">
+        <v>3</v>
+      </c>
+      <c r="AX11">
+        <v>1</v>
+      </c>
+      <c r="AY11">
+        <v>1</v>
+      </c>
+      <c r="AZ11">
+        <v>1</v>
+      </c>
+      <c r="BA11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:71">
       <c r="A12" s="4">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>70</v>
       </c>
       <c r="C12" s="1">
-        <v>117.2</v>
+        <v>11.9</v>
       </c>
       <c r="D12" s="2">
-        <f>HYPERLINK("https://torgi.gov.ru/new/public/lots/lot/22000019850000000011_1/(lotInfo:info)", "22000019850000000011_1")</f>
+        <f>HYPERLINK("https://torgi.gov.ru/new/public/lots/lot/21000025550000000047_1/(lotInfo:info)", "21000025550000000047_1")</f>
         <v>0</v>
       </c>
       <c r="E12" t="s">
-        <v>21</v>
+        <v>83</v>
       </c>
       <c r="F12" s="3">
-        <v>17496.98805460751</v>
+        <v>27030.84033613445</v>
       </c>
       <c r="G12" s="3">
-        <v>2050647</v>
+        <v>321667</v>
+      </c>
+      <c r="H12" t="s">
+        <v>100</v>
       </c>
       <c r="I12" t="s">
-        <v>52</v>
+        <v>124</v>
       </c>
       <c r="J12" t="s">
-        <v>64</v>
+        <v>142</v>
       </c>
       <c r="L12" t="s">
-        <v>74</v>
+        <v>159</v>
       </c>
       <c r="M12" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13">
+        <v>162</v>
+      </c>
+      <c r="N12" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="13" spans="1:71">
       <c r="A13" s="4">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>70</v>
       </c>
       <c r="C13" s="1">
-        <v>237.4</v>
+        <v>10</v>
       </c>
       <c r="D13" s="2">
-        <f>HYPERLINK("https://torgi.gov.ru/new/public/lots/lot/22000019850000000010_1/(lotInfo:info)", "22000019850000000010_1")</f>
+        <f>HYPERLINK("https://torgi.gov.ru/new/public/lots/lot/21000025550000000047_2/(lotInfo:info)", "21000025550000000047_2")</f>
         <v>0</v>
       </c>
       <c r="E13" t="s">
-        <v>22</v>
+        <v>83</v>
       </c>
       <c r="F13" s="3">
-        <v>1578</v>
+        <v>29666.7</v>
       </c>
       <c r="G13" s="3">
-        <v>374617.2</v>
+        <v>296667</v>
       </c>
       <c r="H13" t="s">
-        <v>38</v>
+        <v>101</v>
       </c>
       <c r="I13" t="s">
-        <v>52</v>
+        <v>124</v>
       </c>
       <c r="J13" t="s">
-        <v>65</v>
+        <v>143</v>
       </c>
       <c r="L13" t="s">
-        <v>74</v>
+        <v>159</v>
       </c>
       <c r="M13" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13">
+        <v>162</v>
+      </c>
+      <c r="N13" t="s">
+        <v>170</v>
+      </c>
+      <c r="O13">
+        <v>2</v>
+      </c>
+      <c r="T13">
+        <v>795</v>
+      </c>
+      <c r="U13">
+        <v>3</v>
+      </c>
+      <c r="AD13">
+        <v>1</v>
+      </c>
+      <c r="AG13">
+        <v>1</v>
+      </c>
+      <c r="AW13">
+        <v>3</v>
+      </c>
+      <c r="AX13">
+        <v>1</v>
+      </c>
+      <c r="AY13">
+        <v>1</v>
+      </c>
+      <c r="AZ13">
+        <v>1</v>
+      </c>
+      <c r="BA13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:71">
       <c r="A14" s="4">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>70</v>
       </c>
       <c r="C14" s="1">
-        <v>261.6</v>
+        <v>154.3</v>
       </c>
       <c r="D14" s="2">
-        <f>HYPERLINK("https://torgi.gov.ru/new/public/lots/lot/21000026240000000018_1/(lotInfo:info)", "21000026240000000018_1")</f>
+        <f>HYPERLINK("https://torgi.gov.ru/new/public/lots/lot/21000025550000000046_13/(lotInfo:info)", "21000025550000000046_13")</f>
         <v>0</v>
       </c>
       <c r="E14" t="s">
-        <v>23</v>
+        <v>84</v>
       </c>
       <c r="F14" s="3">
-        <v>35904.12844036697</v>
+        <v>8758.91121192482</v>
       </c>
       <c r="G14" s="3">
-        <v>9392520</v>
+        <v>1351500</v>
       </c>
       <c r="H14" t="s">
+        <v>102</v>
+      </c>
+      <c r="I14" t="s">
+        <v>124</v>
+      </c>
+      <c r="J14" t="s">
+        <v>144</v>
+      </c>
+      <c r="L14" t="s">
+        <v>159</v>
+      </c>
+      <c r="M14" t="s">
+        <v>162</v>
+      </c>
+      <c r="N14" t="s">
+        <v>171</v>
+      </c>
+      <c r="T14">
         <v>39</v>
       </c>
-      <c r="I14" t="s">
-        <v>53</v>
-      </c>
-      <c r="J14" t="s">
-        <v>66</v>
-      </c>
-      <c r="L14" t="s">
-        <v>75</v>
-      </c>
-      <c r="M14" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13">
+      <c r="U14">
+        <v>7</v>
+      </c>
+      <c r="AG14">
+        <v>1</v>
+      </c>
+      <c r="BB14">
+        <v>1</v>
+      </c>
+      <c r="BC14">
+        <v>2</v>
+      </c>
+      <c r="BD14">
+        <v>1</v>
+      </c>
+      <c r="BE14">
+        <v>1</v>
+      </c>
+      <c r="BF14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:71">
       <c r="A15" s="4">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>70</v>
       </c>
       <c r="C15" s="1">
-        <v>46.7</v>
+        <v>138</v>
       </c>
       <c r="D15" s="2">
-        <f>HYPERLINK("https://torgi.gov.ru/new/public/lots/lot/21000026240000000018_4/(lotInfo:info)", "21000026240000000018_4")</f>
+        <f>HYPERLINK("https://torgi.gov.ru/new/public/lots/lot/21000025550000000046_12/(lotInfo:info)", "21000025550000000046_12")</f>
         <v>0</v>
       </c>
       <c r="E15" t="s">
-        <v>24</v>
+        <v>84</v>
       </c>
       <c r="F15" s="3">
-        <v>37284.7965738758</v>
+        <v>8756.644565217392</v>
       </c>
       <c r="G15" s="3">
-        <v>1741200</v>
+        <v>1208416.95</v>
       </c>
       <c r="H15" t="s">
-        <v>40</v>
+        <v>102</v>
       </c>
       <c r="I15" t="s">
-        <v>53</v>
+        <v>124</v>
       </c>
       <c r="J15" t="s">
-        <v>67</v>
+        <v>145</v>
       </c>
       <c r="L15" t="s">
-        <v>75</v>
+        <v>159</v>
       </c>
       <c r="M15" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13">
+        <v>162</v>
+      </c>
+      <c r="N15" t="s">
+        <v>171</v>
+      </c>
+      <c r="T15">
+        <v>39</v>
+      </c>
+      <c r="U15">
+        <v>7</v>
+      </c>
+      <c r="AG15">
+        <v>1</v>
+      </c>
+      <c r="BB15">
+        <v>1</v>
+      </c>
+      <c r="BC15">
+        <v>2</v>
+      </c>
+      <c r="BD15">
+        <v>1</v>
+      </c>
+      <c r="BE15">
+        <v>1</v>
+      </c>
+      <c r="BF15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:71">
       <c r="A16" s="4">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>70</v>
       </c>
       <c r="C16" s="1">
-        <v>53.5</v>
+        <v>126.3</v>
       </c>
       <c r="D16" s="2">
-        <f>HYPERLINK("https://torgi.gov.ru/new/public/lots/lot/21000026240000000018_2/(lotInfo:info)", "21000026240000000018_2")</f>
+        <f>HYPERLINK("https://torgi.gov.ru/new/public/lots/lot/21000025550000000046_11/(lotInfo:info)", "21000025550000000046_11")</f>
         <v>0</v>
       </c>
       <c r="E16" t="s">
-        <v>25</v>
+        <v>84</v>
       </c>
       <c r="F16" s="3">
-        <v>38949.53271028037</v>
+        <v>8317.165874901029</v>
       </c>
       <c r="G16" s="3">
-        <v>2083800</v>
+        <v>1050458.05</v>
       </c>
       <c r="H16" t="s">
-        <v>41</v>
+        <v>103</v>
       </c>
       <c r="I16" t="s">
-        <v>53</v>
+        <v>124</v>
       </c>
       <c r="J16" t="s">
-        <v>68</v>
+        <v>146</v>
       </c>
       <c r="L16" t="s">
-        <v>75</v>
+        <v>159</v>
       </c>
       <c r="M16" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13">
+        <v>162</v>
+      </c>
+      <c r="N16" t="s">
+        <v>172</v>
+      </c>
+      <c r="P16">
+        <v>3</v>
+      </c>
+      <c r="T16">
+        <v>5472</v>
+      </c>
+      <c r="U16">
+        <v>6</v>
+      </c>
+      <c r="AD16">
+        <v>1</v>
+      </c>
+      <c r="AH16">
+        <v>1</v>
+      </c>
+      <c r="AK16">
+        <v>1</v>
+      </c>
+      <c r="AQ16">
+        <v>1</v>
+      </c>
+      <c r="AW16">
+        <v>1</v>
+      </c>
+      <c r="AX16">
+        <v>1</v>
+      </c>
+      <c r="AY16">
+        <v>3</v>
+      </c>
+      <c r="BC16">
+        <v>2</v>
+      </c>
+      <c r="BG16">
+        <v>3</v>
+      </c>
+      <c r="BH16">
+        <v>1</v>
+      </c>
+      <c r="BI16">
+        <v>1</v>
+      </c>
+      <c r="BJ16">
+        <v>1</v>
+      </c>
+      <c r="BK16">
+        <v>1</v>
+      </c>
+      <c r="BL16">
+        <v>2</v>
+      </c>
+      <c r="BM16">
+        <v>1</v>
+      </c>
+      <c r="BN16">
+        <v>1</v>
+      </c>
+      <c r="BO16">
+        <v>1</v>
+      </c>
+      <c r="BP16">
+        <v>2</v>
+      </c>
+      <c r="BQ16">
+        <v>1</v>
+      </c>
+      <c r="BR16">
+        <v>1</v>
+      </c>
+      <c r="BS16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
       <c r="A17" s="4">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>73</v>
       </c>
       <c r="C17" s="1">
-        <v>30.7</v>
+        <v>44.7</v>
       </c>
       <c r="D17" s="2">
-        <f>HYPERLINK("https://torgi.gov.ru/new/public/lots/lot/21000026240000000018_3/(lotInfo:info)", "21000026240000000018_3")</f>
+        <f>HYPERLINK("https://torgi.gov.ru/new/public/lots/lot/21000012500000000015_4/(lotInfo:info)", "21000012500000000015_4")</f>
         <v>0</v>
       </c>
       <c r="E17" t="s">
-        <v>24</v>
+        <v>83</v>
       </c>
       <c r="F17" s="3">
-        <v>37309.44625407166</v>
+        <v>0</v>
       </c>
       <c r="G17" s="3">
-        <v>1145400</v>
+        <v>0</v>
       </c>
       <c r="H17" t="s">
-        <v>42</v>
+        <v>104</v>
       </c>
       <c r="I17" t="s">
-        <v>53</v>
+        <v>125</v>
       </c>
       <c r="J17" t="s">
-        <v>69</v>
+        <v>147</v>
       </c>
       <c r="L17" t="s">
-        <v>75</v>
+        <v>160</v>
       </c>
       <c r="M17" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13">
+        <v>161</v>
+      </c>
+      <c r="N17" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
       <c r="A18" s="4">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>15</v>
+        <v>72</v>
       </c>
       <c r="C18" s="1">
-        <v>60.1</v>
+        <v>3270</v>
       </c>
       <c r="D18" s="2">
-        <f>HYPERLINK("https://torgi.gov.ru/new/public/lots/lot/21000026240000000018_5/(lotInfo:info)", "21000026240000000018_5")</f>
+        <f>HYPERLINK("https://torgi.gov.ru/new/public/lots/lot/21000025550000000044_3/(lotInfo:info)", "21000025550000000044_3")</f>
         <v>0</v>
       </c>
       <c r="E18" t="s">
-        <v>24</v>
+        <v>85</v>
       </c>
       <c r="F18" s="3">
-        <v>37237.93677204659</v>
+        <v>388.3792048929664</v>
       </c>
       <c r="G18" s="3">
-        <v>2238000</v>
+        <v>1270000</v>
       </c>
       <c r="H18" t="s">
-        <v>43</v>
+        <v>105</v>
       </c>
       <c r="I18" t="s">
-        <v>53</v>
+        <v>126</v>
       </c>
       <c r="J18" t="s">
-        <v>70</v>
+        <v>148</v>
       </c>
       <c r="L18" t="s">
-        <v>75</v>
+        <v>159</v>
       </c>
       <c r="M18" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13">
+        <v>162</v>
+      </c>
+      <c r="N18" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
       <c r="A19" s="4">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>16</v>
+        <v>73</v>
       </c>
       <c r="C19" s="1">
-        <v>676.4</v>
+        <v>62.2</v>
       </c>
       <c r="D19" s="2">
-        <f>HYPERLINK("https://torgi.gov.ru/new/public/lots/lot/21000004300000000002_1/(lotInfo:info)", "21000004300000000002_1")</f>
+        <f>HYPERLINK("https://torgi.gov.ru/new/public/lots/lot/22000052780000000006_1/(lotInfo:info)", "22000052780000000006_1")</f>
         <v>0</v>
       </c>
       <c r="E19" t="s">
-        <v>26</v>
+        <v>86</v>
       </c>
       <c r="F19" s="3">
-        <v>16030.01182732111</v>
+        <v>14405.14469453376</v>
       </c>
       <c r="G19" s="3">
-        <v>10842700</v>
+        <v>896000</v>
       </c>
       <c r="H19" t="s">
-        <v>44</v>
+        <v>106</v>
       </c>
       <c r="I19" t="s">
-        <v>54</v>
+        <v>127</v>
       </c>
       <c r="J19" t="s">
-        <v>71</v>
+        <v>149</v>
       </c>
       <c r="L19" t="s">
-        <v>75</v>
+        <v>159</v>
       </c>
       <c r="M19" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13">
+        <v>161</v>
+      </c>
+      <c r="N19" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
       <c r="A20" s="4">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>16</v>
+        <v>72</v>
       </c>
       <c r="C20" s="1">
-        <v>76.59999999999999</v>
+        <v>60.1</v>
       </c>
       <c r="D20" s="2">
-        <f>HYPERLINK("https://torgi.gov.ru/new/public/lots/lot/21000025550000000030_4/(lotInfo:info)", "21000025550000000030_4")</f>
+        <f>HYPERLINK("https://torgi.gov.ru/new/public/lots/lot/21000016520000000004_1/(lotInfo:info)", "21000016520000000004_1")</f>
         <v>0</v>
       </c>
       <c r="E20" t="s">
-        <v>27</v>
+        <v>87</v>
       </c>
       <c r="F20" s="3">
-        <v>28002.28459530026</v>
+        <v>31613.97670549085</v>
       </c>
       <c r="G20" s="3">
-        <v>2144975</v>
+        <v>1900000</v>
       </c>
       <c r="H20" t="s">
-        <v>45</v>
+        <v>107</v>
       </c>
       <c r="I20" t="s">
-        <v>55</v>
+        <v>128</v>
       </c>
       <c r="J20" t="s">
-        <v>72</v>
+        <v>150</v>
       </c>
       <c r="L20" t="s">
-        <v>74</v>
+        <v>159</v>
       </c>
       <c r="M20" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13">
+        <v>161</v>
+      </c>
+      <c r="N20" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
       <c r="A21" s="4">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>16</v>
+        <v>70</v>
       </c>
       <c r="C21" s="1">
-        <v>81.09999999999999</v>
+        <v>156.5</v>
       </c>
       <c r="D21" s="2">
-        <f>HYPERLINK("https://torgi.gov.ru/new/public/lots/lot/21000025550000000030_3/(lotInfo:info)", "21000025550000000030_3")</f>
+        <f>HYPERLINK("https://torgi.gov.ru/new/public/lots/lot/22000089360000000001_1/(lotInfo:info)", "22000089360000000001_1")</f>
         <v>0</v>
       </c>
       <c r="E21" t="s">
-        <v>28</v>
+        <v>88</v>
       </c>
       <c r="F21" s="3">
-        <v>15843.61220715167</v>
+        <v>26747.60383386581</v>
       </c>
       <c r="G21" s="3">
-        <v>1284916.95</v>
+        <v>4186000</v>
       </c>
       <c r="H21" t="s">
-        <v>46</v>
+        <v>108</v>
       </c>
       <c r="I21" t="s">
-        <v>55</v>
-      </c>
-      <c r="J21" t="s">
-        <v>73</v>
+        <v>129</v>
       </c>
       <c r="L21" t="s">
+        <v>159</v>
+      </c>
+      <c r="M21" t="s">
+        <v>161</v>
+      </c>
+      <c r="N21" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="A22" s="4">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
         <v>74</v>
       </c>
-      <c r="M21" t="s">
-        <v>76</v>
+      <c r="C22" s="1">
+        <v>28.9</v>
+      </c>
+      <c r="D22" s="2">
+        <f>HYPERLINK("https://torgi.gov.ru/new/public/lots/lot/22000084990000000003_1/(lotInfo:info)", "22000084990000000003_1")</f>
+        <v>0</v>
+      </c>
+      <c r="E22" t="s">
+        <v>89</v>
+      </c>
+      <c r="F22" s="3">
+        <v>10508.65051903114</v>
+      </c>
+      <c r="G22" s="3">
+        <v>303700</v>
+      </c>
+      <c r="H22" t="s">
+        <v>109</v>
+      </c>
+      <c r="I22" t="s">
+        <v>130</v>
+      </c>
+      <c r="J22" t="s">
+        <v>151</v>
+      </c>
+      <c r="L22" t="s">
+        <v>159</v>
+      </c>
+      <c r="M22" t="s">
+        <v>161</v>
+      </c>
+      <c r="N22" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="A23" s="4">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" s="1">
+        <v>56.1</v>
+      </c>
+      <c r="D23" s="2">
+        <f>HYPERLINK("https://torgi.gov.ru/new/public/lots/lot/22000125930000000001_1/(lotInfo:info)", "22000125930000000001_1")</f>
+        <v>0</v>
+      </c>
+      <c r="E23" t="s">
+        <v>90</v>
+      </c>
+      <c r="F23" s="3">
+        <v>8084.313725490196</v>
+      </c>
+      <c r="G23" s="3">
+        <v>453530</v>
+      </c>
+      <c r="H23" t="s">
+        <v>110</v>
+      </c>
+      <c r="I23" t="s">
+        <v>126</v>
+      </c>
+      <c r="J23" t="s">
+        <v>152</v>
+      </c>
+      <c r="K23" s="3">
+        <v>453530</v>
+      </c>
+      <c r="L23" t="s">
+        <v>159</v>
+      </c>
+      <c r="M23" t="s">
+        <v>161</v>
+      </c>
+      <c r="N23" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
+      <c r="A24" s="4">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>70</v>
+      </c>
+      <c r="C24" s="1">
+        <v>186</v>
+      </c>
+      <c r="D24" s="2">
+        <f>HYPERLINK("https://torgi.gov.ru/new/public/lots/lot/21000025550000000040_8/(lotInfo:info)", "21000025550000000040_8")</f>
+        <v>0</v>
+      </c>
+      <c r="E24" t="s">
+        <v>83</v>
+      </c>
+      <c r="F24" s="3">
+        <v>44708.77956989247</v>
+      </c>
+      <c r="G24" s="3">
+        <v>8315833</v>
+      </c>
+      <c r="H24" t="s">
+        <v>111</v>
+      </c>
+      <c r="I24" t="s">
+        <v>131</v>
+      </c>
+      <c r="J24" t="s">
+        <v>153</v>
+      </c>
+      <c r="L24" t="s">
+        <v>159</v>
+      </c>
+      <c r="M24" t="s">
+        <v>162</v>
+      </c>
+      <c r="N24" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
+      <c r="A25" s="4">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>70</v>
+      </c>
+      <c r="C25" s="1">
+        <v>154.6</v>
+      </c>
+      <c r="D25" s="2">
+        <f>HYPERLINK("https://torgi.gov.ru/new/public/lots/lot/21000025550000000040_6/(lotInfo:info)", "21000025550000000040_6")</f>
+        <v>0</v>
+      </c>
+      <c r="E25" t="s">
+        <v>83</v>
+      </c>
+      <c r="F25" s="3">
+        <v>37106.51358344114</v>
+      </c>
+      <c r="G25" s="3">
+        <v>5736667</v>
+      </c>
+      <c r="H25" t="s">
+        <v>112</v>
+      </c>
+      <c r="I25" t="s">
+        <v>131</v>
+      </c>
+      <c r="J25" t="s">
+        <v>154</v>
+      </c>
+      <c r="L25" t="s">
+        <v>159</v>
+      </c>
+      <c r="M25" t="s">
+        <v>162</v>
+      </c>
+      <c r="N25" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14">
+      <c r="A26" s="4">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>70</v>
+      </c>
+      <c r="C26" s="1">
+        <v>194</v>
+      </c>
+      <c r="D26" s="2">
+        <f>HYPERLINK("https://torgi.gov.ru/new/public/lots/lot/21000025550000000040_5/(lotInfo:info)", "21000025550000000040_5")</f>
+        <v>0</v>
+      </c>
+      <c r="E26" t="s">
+        <v>83</v>
+      </c>
+      <c r="F26" s="3">
+        <v>44707.90206185567</v>
+      </c>
+      <c r="G26" s="3">
+        <v>8673333</v>
+      </c>
+      <c r="H26" t="s">
+        <v>113</v>
+      </c>
+      <c r="I26" t="s">
+        <v>131</v>
+      </c>
+      <c r="J26" t="s">
+        <v>155</v>
+      </c>
+      <c r="L26" t="s">
+        <v>159</v>
+      </c>
+      <c r="M26" t="s">
+        <v>162</v>
+      </c>
+      <c r="N26" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14">
+      <c r="A27" s="4">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>70</v>
+      </c>
+      <c r="C27" s="1">
+        <v>143.6</v>
+      </c>
+      <c r="D27" s="2">
+        <f>HYPERLINK("https://torgi.gov.ru/new/public/lots/lot/21000025550000000040_7/(lotInfo:info)", "21000025550000000040_7")</f>
+        <v>0</v>
+      </c>
+      <c r="E27" t="s">
+        <v>83</v>
+      </c>
+      <c r="F27" s="3">
+        <v>37523.21030640668</v>
+      </c>
+      <c r="G27" s="3">
+        <v>5388333</v>
+      </c>
+      <c r="H27" t="s">
+        <v>114</v>
+      </c>
+      <c r="I27" t="s">
+        <v>131</v>
+      </c>
+      <c r="J27" t="s">
+        <v>156</v>
+      </c>
+      <c r="L27" t="s">
+        <v>159</v>
+      </c>
+      <c r="M27" t="s">
+        <v>162</v>
+      </c>
+      <c r="N27" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14">
+      <c r="A28" s="4">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>70</v>
+      </c>
+      <c r="C28" s="1">
+        <v>126.2</v>
+      </c>
+      <c r="D28" s="2">
+        <f>HYPERLINK("https://torgi.gov.ru/new/public/lots/lot/21000025550000000040_9/(lotInfo:info)", "21000025550000000040_9")</f>
+        <v>0</v>
+      </c>
+      <c r="E28" t="s">
+        <v>83</v>
+      </c>
+      <c r="F28" s="3">
+        <v>37731.11727416798</v>
+      </c>
+      <c r="G28" s="3">
+        <v>4761667</v>
+      </c>
+      <c r="H28" t="s">
+        <v>115</v>
+      </c>
+      <c r="I28" t="s">
+        <v>131</v>
+      </c>
+      <c r="J28" t="s">
+        <v>157</v>
+      </c>
+      <c r="L28" t="s">
+        <v>159</v>
+      </c>
+      <c r="M28" t="s">
+        <v>162</v>
+      </c>
+      <c r="N28" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14">
+      <c r="A29" s="4">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>70</v>
+      </c>
+      <c r="C29" s="1">
+        <v>22.9</v>
+      </c>
+      <c r="D29" s="2">
+        <f>HYPERLINK("https://torgi.gov.ru/new/public/lots/lot/21000025550000000040_17/(lotInfo:info)", "21000025550000000040_17")</f>
+        <v>0</v>
+      </c>
+      <c r="E29" t="s">
+        <v>83</v>
+      </c>
+      <c r="F29" s="3">
+        <v>10516.7248908297</v>
+      </c>
+      <c r="G29" s="3">
+        <v>240833</v>
+      </c>
+      <c r="H29" t="s">
+        <v>116</v>
+      </c>
+      <c r="I29" t="s">
+        <v>131</v>
+      </c>
+      <c r="J29" t="s">
+        <v>158</v>
+      </c>
+      <c r="L29" t="s">
+        <v>159</v>
+      </c>
+      <c r="M29" t="s">
+        <v>162</v>
+      </c>
+      <c r="N29" t="s">
+        <v>166</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
optimization get data from osm (all obj in region)
</commit_message>
<xml_diff>
--- a/torgi/output.xlsx
+++ b/torgi/output.xlsx
@@ -17,12 +17,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="#\ ##0.0\ \м\2"/>
     <numFmt numFmtId="165" formatCode="#\ ###\ ##0\ \₽"/>
-    <numFmt numFmtId="166" formatCode="_-* # ##0.00 ₽_-;-* # ##0.00 ₽_-"/>
+    <numFmt numFmtId="166" formatCode="_-* #\ ##0.00\ \₽_-;\-* #\ ##0.00\ \₽_-"/>
+    <numFmt numFmtId="167" formatCode="_-* # ##0.00 ₽_-;-* # ##0.00 ₽_-"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -45,6 +46,18 @@
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <color rgb="FF0000FF"/>
+      <sz val="11"/>
+      <u val="single"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <color rgb="FF0000FF"/>
+      <sz val="11"/>
+      <u val="single"/>
     </font>
     <font>
       <color rgb="000000FF"/>
@@ -86,7 +99,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -96,6 +109,16 @@
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -473,10 +496,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S71"/>
+  <dimension ref="A1:U71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="H74" sqref="H74"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="T1" sqref="T1:U1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -540,10 +563,8 @@
           <t>Кадастровый номер</t>
         </is>
       </c>
-      <c r="K1" s="4" t="inlineStr">
-        <is>
-          <t>Cтоимость чел/кв.м</t>
-        </is>
+      <c r="K1" s="7" t="n">
+        <v>2.2</v>
       </c>
       <c r="L1" s="4" t="inlineStr">
         <is>
@@ -560,21 +581,12 @@
           <t>Координаты</t>
         </is>
       </c>
-      <c r="O1" s="4" t="inlineStr">
-        <is>
-          <t>Жителей в округе</t>
-        </is>
-      </c>
-      <c r="P1" s="4" t="inlineStr">
-        <is>
-          <t>Коммерческих объектов</t>
-        </is>
-      </c>
-      <c r="Q1" s="4" t="inlineStr">
-        <is>
-          <t>Описание коммерческих объектов</t>
-        </is>
-      </c>
+      <c r="Q1" s="8">
+        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/54.93757_48.83902.json", "54.93757_48.83902.json")</f>
+        <v/>
+      </c>
+      <c r="T1" s="4" t="n"/>
+      <c r="U1" s="4" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="4" t="n">
@@ -618,7 +630,7 @@
           <t>16:38:130101:773</t>
         </is>
       </c>
-      <c r="K2" s="5" t="n">
+      <c r="K2" s="11" t="n">
         <v>2.2</v>
       </c>
       <c r="L2" t="inlineStr">
@@ -646,15 +658,25 @@
           <t>6</t>
         </is>
       </c>
-      <c r="Q2" s="6">
-        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/54.93757_ 48.83902.json", "54.93757_ 48.83902.json")</f>
+      <c r="Q2" s="12">
+        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/54.93757_48.83902.json", "54.93757_48.83902.json")</f>
         <v/>
       </c>
       <c r="R2" t="n">
         <v>393</v>
       </c>
-      <c r="S2" s="5" t="n">
+      <c r="S2" s="9" t="n">
         <v>2.96</v>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>528</t>
+        </is>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -699,7 +721,7 @@
           <t>21:01:010607:257</t>
         </is>
       </c>
-      <c r="K3" s="5" t="n">
+      <c r="K3" s="11" t="n">
         <v>7.3</v>
       </c>
       <c r="L3" t="inlineStr">
@@ -726,15 +748,25 @@
           <t>33</t>
         </is>
       </c>
-      <c r="Q3" s="6">
-        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/56.125862_ 47.21173.json", "56.125862_ 47.21173.json")</f>
+      <c r="Q3" s="12">
+        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/56.125862_47.21173.json", "56.125862_47.21173.json")</f>
         <v/>
       </c>
       <c r="R3" t="n">
         <v>2663</v>
       </c>
-      <c r="S3" s="5" t="n">
+      <c r="S3" s="9" t="n">
         <v>4.82</v>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>1758</t>
+        </is>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -779,7 +811,7 @@
           <t xml:space="preserve">77:03:0005014:11807 </t>
         </is>
       </c>
-      <c r="K4" s="5" t="n">
+      <c r="K4" s="11" t="n">
         <v>6.93</v>
       </c>
       <c r="L4" t="inlineStr">
@@ -806,15 +838,25 @@
           <t>104</t>
         </is>
       </c>
-      <c r="Q4" s="6">
-        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.79225_ 37.812588.json", "55.79225_ 37.812588.json")</f>
+      <c r="Q4" s="12">
+        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.79225_37.812588.json", "55.79225_37.812588.json")</f>
         <v/>
       </c>
       <c r="R4" t="n">
         <v>8197</v>
       </c>
-      <c r="S4" s="5" t="n">
+      <c r="S4" s="9" t="n">
         <v>13.55</v>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>16035</t>
+        </is>
+      </c>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>104</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -859,7 +901,7 @@
           <t>50:43:0030304:1156</t>
         </is>
       </c>
-      <c r="K5" s="5" t="n">
+      <c r="K5" s="11" t="n">
         <v>7.59</v>
       </c>
       <c r="L5" t="inlineStr">
@@ -886,15 +928,25 @@
           <t>37</t>
         </is>
       </c>
-      <c r="Q5" s="6">
-        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.97189_ 37.9131.json", "55.97189_ 37.9131.json")</f>
+      <c r="Q5" s="12">
+        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.97189_37.9131.json", "55.97189_37.9131.json")</f>
         <v/>
       </c>
       <c r="R5" t="n">
         <v>3785</v>
       </c>
-      <c r="S5" s="5" t="n">
+      <c r="S5" s="9" t="n">
         <v>7.51</v>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>3744</t>
+        </is>
+      </c>
+      <c r="U5" t="inlineStr">
+        <is>
+          <t>37</t>
+        </is>
       </c>
     </row>
     <row r="6">
@@ -939,7 +991,7 @@
           <t>50:57:0000000:7243</t>
         </is>
       </c>
-      <c r="K6" s="5" t="n">
+      <c r="K6" s="11" t="n">
         <v>23.82</v>
       </c>
       <c r="L6" t="inlineStr">
@@ -966,15 +1018,25 @@
           <t>8</t>
         </is>
       </c>
-      <c r="Q6" s="6">
-        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.107061_ 38.743359.json", "55.107061_ 38.743359.json")</f>
+      <c r="Q6" s="12">
+        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.107061_38.743359.json", "55.107061_38.743359.json")</f>
         <v/>
       </c>
       <c r="R6" t="n">
         <v>2272</v>
       </c>
-      <c r="S6" s="5" t="n">
+      <c r="S6" s="9" t="n">
         <v>13.88</v>
+      </c>
+      <c r="T6" t="inlineStr">
+        <is>
+          <t>1324</t>
+        </is>
+      </c>
+      <c r="U6" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
       </c>
     </row>
     <row r="7">
@@ -1019,7 +1081,7 @@
           <t>50:35:0030405:1682</t>
         </is>
       </c>
-      <c r="K7" s="5" t="n">
+      <c r="K7" s="11" t="n">
         <v>9.609999999999999</v>
       </c>
       <c r="L7" t="inlineStr">
@@ -1046,15 +1108,25 @@
           <t>3</t>
         </is>
       </c>
-      <c r="Q7" s="6">
-        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/54.849313_ 39.305731.json", "54.849313_ 39.305731.json")</f>
+      <c r="Q7" s="12">
+        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/54.849313_39.305731.json", "54.849313_39.305731.json")</f>
         <v/>
       </c>
       <c r="R7" t="n">
         <v>144</v>
       </c>
-      <c r="S7" s="5" t="n">
+      <c r="S7" s="9" t="n">
         <v>62.52</v>
+      </c>
+      <c r="T7" t="inlineStr">
+        <is>
+          <t>937</t>
+        </is>
+      </c>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
     </row>
     <row r="8">
@@ -1099,7 +1171,7 @@
           <t>16:50:000000:10993</t>
         </is>
       </c>
-      <c r="K8" s="5" t="inlineStr"/>
+      <c r="K8" s="9" t="n"/>
       <c r="L8" t="inlineStr">
         <is>
           <t>EA</t>
@@ -1108,20 +1180,6 @@
       <c r="M8" t="inlineStr">
         <is>
           <t>М</t>
-        </is>
-      </c>
-      <c r="N8" s="2">
-        <f>HYPERLINK("https://yandex.ru/maps/?&amp;text=47.52033, 42.190483", "47.52033, 42.190483")</f>
-        <v/>
-      </c>
-      <c r="O8" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="P8" t="inlineStr">
-        <is>
-          <t>0</t>
         </is>
       </c>
       <c r="Q8" s="6">
@@ -1131,7 +1189,7 @@
       <c r="R8" t="n">
         <v>2929</v>
       </c>
-      <c r="S8" s="5" t="n">
+      <c r="S8" s="9" t="n">
         <v>2.29</v>
       </c>
     </row>
@@ -1177,7 +1235,7 @@
           <t>16:50:011816:115</t>
         </is>
       </c>
-      <c r="K9" s="5" t="n">
+      <c r="K9" s="11" t="n">
         <v>18.35</v>
       </c>
       <c r="L9" t="inlineStr">
@@ -1204,15 +1262,25 @@
           <t>81</t>
         </is>
       </c>
-      <c r="Q9" s="6">
-        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.784577_ 49.109118.json", "55.784577_ 49.109118.json")</f>
+      <c r="Q9" s="12">
+        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.784577_49.109118.json", "55.784577_49.109118.json")</f>
         <v/>
       </c>
       <c r="R9" t="n">
         <v>4266</v>
       </c>
-      <c r="S9" s="5" t="n">
+      <c r="S9" s="9" t="n">
         <v>10.79</v>
+      </c>
+      <c r="T9" t="inlineStr">
+        <is>
+          <t>2508</t>
+        </is>
+      </c>
+      <c r="U9" t="inlineStr">
+        <is>
+          <t>81</t>
+        </is>
       </c>
     </row>
     <row r="10">
@@ -1257,7 +1325,7 @@
           <t xml:space="preserve">77:01:0006007:3888 </t>
         </is>
       </c>
-      <c r="K10" s="5" t="n">
+      <c r="K10" s="11" t="n">
         <v>4.24</v>
       </c>
       <c r="L10" t="inlineStr">
@@ -1284,15 +1352,25 @@
           <t>156</t>
         </is>
       </c>
-      <c r="Q10" s="6">
-        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.716473_ 37.620393.json", "55.716473_ 37.620393.json")</f>
+      <c r="Q10" s="12">
+        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.716473_37.620393.json", "55.716473_37.620393.json")</f>
         <v/>
       </c>
       <c r="R10" t="n">
         <v>6298</v>
       </c>
-      <c r="S10" s="5" t="n">
+      <c r="S10" s="9" t="n">
         <v>7.68</v>
+      </c>
+      <c r="T10" t="inlineStr">
+        <is>
+          <t>11418</t>
+        </is>
+      </c>
+      <c r="U10" t="inlineStr">
+        <is>
+          <t>156</t>
+        </is>
       </c>
     </row>
     <row r="11">
@@ -1337,7 +1415,7 @@
           <t>77:08:0002022:3598</t>
         </is>
       </c>
-      <c r="K11" s="5" t="n">
+      <c r="K11" s="11" t="n">
         <v>17.52</v>
       </c>
       <c r="L11" t="inlineStr">
@@ -1364,15 +1442,25 @@
           <t>103</t>
         </is>
       </c>
-      <c r="Q11" s="6">
-        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.834153_ 37.356441.json", "55.834153_ 37.356441.json")</f>
+      <c r="Q11" s="12">
+        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.834153_37.356441.json", "55.834153_37.356441.json")</f>
         <v/>
       </c>
       <c r="R11" t="n">
         <v>9513</v>
       </c>
-      <c r="S11" s="5" t="n">
+      <c r="S11" s="9" t="n">
         <v>15.66</v>
+      </c>
+      <c r="T11" t="inlineStr">
+        <is>
+          <t>8502</t>
+        </is>
+      </c>
+      <c r="U11" t="inlineStr">
+        <is>
+          <t>103</t>
+        </is>
       </c>
     </row>
     <row r="12">
@@ -1417,7 +1505,7 @@
           <t>77:10:0000000:2691</t>
         </is>
       </c>
-      <c r="K12" s="5" t="n">
+      <c r="K12" s="11" t="n">
         <v>10.31</v>
       </c>
       <c r="L12" t="inlineStr">
@@ -1444,15 +1532,25 @@
           <t>38</t>
         </is>
       </c>
-      <c r="Q12" s="6">
-        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/56.008817_ 37.206737.json", "56.008817_ 37.206737.json")</f>
+      <c r="Q12" s="12">
+        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/56.008817_37.206737.json", "56.008817_37.206737.json")</f>
         <v/>
       </c>
       <c r="R12" t="n">
         <v>2987</v>
       </c>
-      <c r="S12" s="5" t="n">
+      <c r="S12" s="9" t="n">
         <v>31</v>
+      </c>
+      <c r="T12" t="inlineStr">
+        <is>
+          <t>8982</t>
+        </is>
+      </c>
+      <c r="U12" t="inlineStr">
+        <is>
+          <t>38</t>
+        </is>
       </c>
     </row>
     <row r="13">
@@ -1497,7 +1595,7 @@
           <t>50:58:0020101:155</t>
         </is>
       </c>
-      <c r="K13" s="5" t="n">
+      <c r="K13" s="11" t="n">
         <v>13.42</v>
       </c>
       <c r="L13" t="inlineStr">
@@ -1524,15 +1622,25 @@
           <t>10</t>
         </is>
       </c>
-      <c r="Q13" s="6">
-        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/54.933_ 37.37951.json", "54.933_ 37.37951.json")</f>
+      <c r="Q13" s="12">
+        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/54.933_37.37951.json", "54.933_37.37951.json")</f>
         <v/>
       </c>
       <c r="R13" t="n">
         <v>2912</v>
       </c>
-      <c r="S13" s="5" t="n">
+      <c r="S13" s="9" t="n">
         <v>7.31</v>
+      </c>
+      <c r="T13" t="inlineStr">
+        <is>
+          <t>1587</t>
+        </is>
+      </c>
+      <c r="U13" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
       </c>
     </row>
     <row r="14">
@@ -1577,7 +1685,7 @@
           <t>77:03:0005014:11774</t>
         </is>
       </c>
-      <c r="K14" s="5" t="n">
+      <c r="K14" s="11" t="n">
         <v>4.13</v>
       </c>
       <c r="L14" t="inlineStr">
@@ -1604,15 +1712,25 @@
           <t>98</t>
         </is>
       </c>
-      <c r="Q14" s="6">
-        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.7912776_ 37.7954093.json", "55.7912776_ 37.7954093.json")</f>
+      <c r="Q14" s="12">
+        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.7912776_37.7954093.json", "55.7912776_37.7954093.json")</f>
         <v/>
       </c>
       <c r="R14" t="n">
         <v>4636</v>
       </c>
-      <c r="S14" s="5" t="n">
+      <c r="S14" s="9" t="n">
         <v>15.06</v>
+      </c>
+      <c r="T14" t="inlineStr">
+        <is>
+          <t>16920</t>
+        </is>
+      </c>
+      <c r="U14" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
       </c>
     </row>
     <row r="15">
@@ -1657,7 +1775,7 @@
           <t>50:17:0011505:498</t>
         </is>
       </c>
-      <c r="K15" s="5" t="n">
+      <c r="K15" s="11" t="n">
         <v>15.02</v>
       </c>
       <c r="L15" t="inlineStr">
@@ -1684,15 +1802,25 @@
           <t>24</t>
         </is>
       </c>
-      <c r="Q15" s="6">
-        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.868945_ 38.782292.json", "55.868945_ 38.782292.json")</f>
+      <c r="Q15" s="12">
+        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.868945_38.782292.json", "55.868945_38.782292.json")</f>
         <v/>
       </c>
       <c r="R15" t="n">
         <v>1628</v>
       </c>
-      <c r="S15" s="5" t="n">
+      <c r="S15" s="9" t="n">
         <v>25.07</v>
+      </c>
+      <c r="T15" t="inlineStr">
+        <is>
+          <t>2718</t>
+        </is>
+      </c>
+      <c r="U15" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
       </c>
     </row>
     <row r="16">
@@ -1737,7 +1865,7 @@
           <t>50:58:0100402:377</t>
         </is>
       </c>
-      <c r="K16" s="5" t="n">
+      <c r="K16" s="11" t="n">
         <v>10.62</v>
       </c>
       <c r="L16" t="inlineStr">
@@ -1764,15 +1892,25 @@
           <t>59</t>
         </is>
       </c>
-      <c r="Q16" s="6">
-        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/54.915839_ 37.421874.json", "54.915839_ 37.421874.json")</f>
+      <c r="Q16" s="12">
+        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/54.915839_37.421874.json", "54.915839_37.421874.json")</f>
         <v/>
       </c>
       <c r="R16" t="n">
         <v>3053</v>
       </c>
-      <c r="S16" s="5" t="n">
+      <c r="S16" s="9" t="n">
         <v>10.77</v>
+      </c>
+      <c r="T16" t="inlineStr">
+        <is>
+          <t>3096</t>
+        </is>
+      </c>
+      <c r="U16" t="inlineStr">
+        <is>
+          <t>59</t>
+        </is>
       </c>
     </row>
     <row r="17">
@@ -1817,7 +1955,7 @@
           <t xml:space="preserve">12:13:0990117:580, </t>
         </is>
       </c>
-      <c r="K17" s="5" t="n">
+      <c r="K17" s="11" t="n">
         <v>0.98</v>
       </c>
       <c r="L17" t="inlineStr">
@@ -1844,15 +1982,25 @@
           <t>4</t>
         </is>
       </c>
-      <c r="Q17" s="6">
-        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/56.437214_ 49.019527.json", "56.437214_ 49.019527.json")</f>
+      <c r="Q17" s="12">
+        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/56.437214_49.019527.json", "56.437214_49.019527.json")</f>
         <v/>
       </c>
       <c r="R17" t="n">
         <v>1244</v>
       </c>
-      <c r="S17" s="5" t="n">
+      <c r="S17" s="9" t="n">
         <v>1.81</v>
+      </c>
+      <c r="T17" t="inlineStr">
+        <is>
+          <t>2286</t>
+        </is>
+      </c>
+      <c r="U17" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
       </c>
     </row>
     <row r="18">
@@ -1897,7 +2045,7 @@
           <t>50:53:0020103:2581</t>
         </is>
       </c>
-      <c r="K18" s="5" t="n">
+      <c r="K18" s="11" t="n">
         <v>4.74</v>
       </c>
       <c r="L18" t="inlineStr">
@@ -1924,15 +2072,25 @@
           <t>28</t>
         </is>
       </c>
-      <c r="Q18" s="6">
-        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.574894_ 37.900665.json", "55.574894_ 37.900665.json")</f>
+      <c r="Q18" s="12">
+        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.574894_37.900665.json", "55.574894_37.900665.json")</f>
         <v/>
       </c>
       <c r="R18" t="n">
         <v>4687</v>
       </c>
-      <c r="S18" s="5" t="n">
+      <c r="S18" s="9" t="n">
         <v>6.91</v>
+      </c>
+      <c r="T18" t="inlineStr">
+        <is>
+          <t>6834</t>
+        </is>
+      </c>
+      <c r="U18" t="inlineStr">
+        <is>
+          <t>28</t>
+        </is>
       </c>
     </row>
     <row r="19">
@@ -1977,7 +2135,7 @@
           <t>50:53:0010107:1524</t>
         </is>
       </c>
-      <c r="K19" s="5" t="n">
+      <c r="K19" s="11" t="n">
         <v>8.140000000000001</v>
       </c>
       <c r="L19" t="inlineStr">
@@ -2004,15 +2162,25 @@
           <t>43</t>
         </is>
       </c>
-      <c r="Q19" s="6">
-        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.576645_ 37.908356.json", "55.576645_ 37.908356.json")</f>
+      <c r="Q19" s="12">
+        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.576645_37.908356.json", "55.576645_37.908356.json")</f>
         <v/>
       </c>
       <c r="R19" t="n">
         <v>3482</v>
       </c>
-      <c r="S19" s="5" t="n">
+      <c r="S19" s="9" t="n">
         <v>16.23</v>
+      </c>
+      <c r="T19" t="inlineStr">
+        <is>
+          <t>6939</t>
+        </is>
+      </c>
+      <c r="U19" t="inlineStr">
+        <is>
+          <t>43</t>
+        </is>
       </c>
     </row>
     <row r="20">
@@ -2057,7 +2225,7 @@
           <t xml:space="preserve">58:05:0160203:870, </t>
         </is>
       </c>
-      <c r="K20" s="5" t="n">
+      <c r="K20" s="11" t="n">
         <v>14.12</v>
       </c>
       <c r="L20" t="inlineStr">
@@ -2084,15 +2252,25 @@
           <t>3</t>
         </is>
       </c>
-      <c r="Q20" s="6">
-        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/53.208954_ 45.305813.json", "53.208954_ 45.305813.json")</f>
+      <c r="Q20" s="12">
+        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/53.208954_45.305813.json", "53.208954_45.305813.json")</f>
         <v/>
       </c>
       <c r="R20" t="n">
         <v>323</v>
       </c>
-      <c r="S20" s="5" t="n">
+      <c r="S20" s="9" t="n">
         <v>67.15000000000001</v>
+      </c>
+      <c r="T20" t="inlineStr">
+        <is>
+          <t>1536</t>
+        </is>
+      </c>
+      <c r="U20" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
     </row>
     <row r="21">
@@ -2137,7 +2315,7 @@
           <t xml:space="preserve">77:06:0008003:1052, </t>
         </is>
       </c>
-      <c r="K21" s="5" t="n">
+      <c r="K21" s="11" t="n">
         <v>34.86</v>
       </c>
       <c r="L21" t="inlineStr">
@@ -2164,15 +2342,25 @@
           <t>45</t>
         </is>
       </c>
-      <c r="Q21" s="6">
-        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.649144_ 37.534918.json", "55.649144_ 37.534918.json")</f>
+      <c r="Q21" s="12">
+        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.649144_37.534918.json", "55.649144_37.534918.json")</f>
         <v/>
       </c>
       <c r="R21" t="n">
         <v>15589</v>
       </c>
-      <c r="S21" s="5" t="n">
+      <c r="S21" s="9" t="n">
         <v>8.970000000000001</v>
+      </c>
+      <c r="T21" t="inlineStr">
+        <is>
+          <t>4011</t>
+        </is>
+      </c>
+      <c r="U21" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
       </c>
     </row>
     <row r="22">
@@ -2217,7 +2405,7 @@
           <t>77:09:0003018:10762</t>
         </is>
       </c>
-      <c r="K22" s="5" t="n">
+      <c r="K22" s="11" t="n">
         <v>27.56</v>
       </c>
       <c r="L22" t="inlineStr">
@@ -2244,15 +2432,25 @@
           <t>148</t>
         </is>
       </c>
-      <c r="Q22" s="6">
-        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.816696_ 37.50204.json", "55.816696_ 37.50204.json")</f>
+      <c r="Q22" s="12">
+        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.816696_37.50204.json", "55.816696_37.50204.json")</f>
         <v/>
       </c>
       <c r="R22" t="n">
         <v>9044</v>
       </c>
-      <c r="S22" s="5" t="n">
+      <c r="S22" s="9" t="n">
         <v>17.68</v>
+      </c>
+      <c r="T22" t="inlineStr">
+        <is>
+          <t>5802</t>
+        </is>
+      </c>
+      <c r="U22" t="inlineStr">
+        <is>
+          <t>148</t>
+        </is>
       </c>
     </row>
     <row r="23">
@@ -2297,7 +2495,7 @@
           <t>16:05:010504:438</t>
         </is>
       </c>
-      <c r="K23" s="5" t="n">
+      <c r="K23" s="11" t="n">
         <v>23.75</v>
       </c>
       <c r="L23" t="inlineStr">
@@ -2324,15 +2522,25 @@
           <t>18</t>
         </is>
       </c>
-      <c r="Q23" s="6">
-        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.30253_ 50.10958.json", "55.30253_ 50.10958.json")</f>
+      <c r="Q23" s="12">
+        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.30253_50.10958.json", "55.30253_50.10958.json")</f>
         <v/>
       </c>
       <c r="R23" t="n">
         <v>906</v>
       </c>
-      <c r="S23" s="5" t="n">
+      <c r="S23" s="9" t="n">
         <v>23.75</v>
+      </c>
+      <c r="T23" t="inlineStr">
+        <is>
+          <t>906</t>
+        </is>
+      </c>
+      <c r="U23" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
       </c>
     </row>
     <row r="24">
@@ -2377,7 +2585,7 @@
           <t xml:space="preserve">58:34:0010141:710, </t>
         </is>
       </c>
-      <c r="K24" s="5" t="n">
+      <c r="K24" s="11" t="n">
         <v>6.91</v>
       </c>
       <c r="L24" t="inlineStr">
@@ -2404,15 +2612,25 @@
           <t>35</t>
         </is>
       </c>
-      <c r="Q24" s="6">
-        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/53.187823_ 45.174578.json", "53.187823_ 45.174578.json")</f>
+      <c r="Q24" s="12">
+        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/53.187823_45.174578.json", "53.187823_45.174578.json")</f>
         <v/>
       </c>
       <c r="R24" t="n">
         <v>3155</v>
       </c>
-      <c r="S24" s="5" t="n">
+      <c r="S24" s="9" t="n">
         <v>16.75</v>
+      </c>
+      <c r="T24" t="inlineStr">
+        <is>
+          <t>7651</t>
+        </is>
+      </c>
+      <c r="U24" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
       </c>
     </row>
     <row r="25">
@@ -2457,7 +2675,7 @@
           <t>21:02:000000:32513</t>
         </is>
       </c>
-      <c r="K25" s="5" t="n">
+      <c r="K25" s="11" t="n">
         <v>224.59</v>
       </c>
       <c r="L25" t="inlineStr">
@@ -2484,15 +2702,25 @@
           <t>14</t>
         </is>
       </c>
-      <c r="Q25" s="6">
-        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/56.07907_ 47.506935.json", "56.07907_ 47.506935.json")</f>
+      <c r="Q25" s="12">
+        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/56.07907_47.506935.json", "56.07907_47.506935.json")</f>
         <v/>
       </c>
       <c r="R25" t="n">
         <v>3527</v>
       </c>
-      <c r="S25" s="5" t="n">
+      <c r="S25" s="9" t="n">
         <v>2.48</v>
+      </c>
+      <c r="T25" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="U25" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
       </c>
     </row>
     <row r="26">
@@ -2537,7 +2765,7 @@
           <t>21:02:000000:32517</t>
         </is>
       </c>
-      <c r="K26" s="5" t="n">
+      <c r="K26" s="11" t="n">
         <v>224.53</v>
       </c>
       <c r="L26" t="inlineStr">
@@ -2564,15 +2792,25 @@
           <t>14</t>
         </is>
       </c>
-      <c r="Q26" s="6">
-        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/56.07907_ 47.506935.json", "56.07907_ 47.506935.json")</f>
+      <c r="Q26" s="12">
+        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/56.07907_47.506935.json", "56.07907_47.506935.json")</f>
         <v/>
       </c>
       <c r="R26" t="n">
         <v>3527</v>
       </c>
-      <c r="S26" s="5" t="n">
+      <c r="S26" s="9" t="n">
         <v>2.48</v>
+      </c>
+      <c r="T26" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="U26" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
       </c>
     </row>
     <row r="27">
@@ -2617,7 +2855,7 @@
           <t>21:01:010103:544</t>
         </is>
       </c>
-      <c r="K27" s="5" t="n">
+      <c r="K27" s="11" t="n">
         <v>1.52</v>
       </c>
       <c r="L27" t="inlineStr">
@@ -2644,15 +2882,25 @@
           <t>37</t>
         </is>
       </c>
-      <c r="Q27" s="6">
-        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/56.15064_ 47.183184.json", "56.15064_ 47.183184.json")</f>
+      <c r="Q27" s="12">
+        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/56.15064_47.183184.json", "56.15064_47.183184.json")</f>
         <v/>
       </c>
       <c r="R27" t="n">
         <v>2412</v>
       </c>
-      <c r="S27" s="5" t="n">
+      <c r="S27" s="9" t="n">
         <v>3.45</v>
+      </c>
+      <c r="T27" t="inlineStr">
+        <is>
+          <t>5472</t>
+        </is>
+      </c>
+      <c r="U27" t="inlineStr">
+        <is>
+          <t>37</t>
+        </is>
       </c>
     </row>
     <row r="28">
@@ -2697,7 +2945,7 @@
           <t>77:01:0003008:3576</t>
         </is>
       </c>
-      <c r="K28" s="5" t="n">
+      <c r="K28" s="11" t="n">
         <v>7.17</v>
       </c>
       <c r="L28" t="inlineStr">
@@ -2724,15 +2972,25 @@
           <t>240</t>
         </is>
       </c>
-      <c r="Q28" s="6">
-        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.7645572_ 37.6569216.json", "55.7645572_ 37.6569216.json")</f>
+      <c r="Q28" s="12">
+        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.7645572_37.6569216.json", "55.7645572_37.6569216.json")</f>
         <v/>
       </c>
       <c r="R28" t="n">
         <v>9190</v>
       </c>
-      <c r="S28" s="5" t="n">
+      <c r="S28" s="9" t="n">
         <v>9.83</v>
+      </c>
+      <c r="T28" t="inlineStr">
+        <is>
+          <t>12602</t>
+        </is>
+      </c>
+      <c r="U28" t="inlineStr">
+        <is>
+          <t>240</t>
+        </is>
       </c>
     </row>
     <row r="29">
@@ -2777,7 +3035,7 @@
           <t>77:09:0002021:6695</t>
         </is>
       </c>
-      <c r="K29" s="5" t="n">
+      <c r="K29" s="11" t="n">
         <v>18.18</v>
       </c>
       <c r="L29" t="inlineStr">
@@ -2804,15 +3062,25 @@
           <t>67</t>
         </is>
       </c>
-      <c r="Q29" s="6">
-        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.8738384_ 37.5390459.json", "55.8738384_ 37.5390459.json")</f>
+      <c r="Q29" s="12">
+        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.8738384_37.5390459.json", "55.8738384_37.5390459.json")</f>
         <v/>
       </c>
       <c r="R29" t="n">
         <v>10984</v>
       </c>
-      <c r="S29" s="5" t="n">
+      <c r="S29" s="9" t="n">
         <v>13.49</v>
+      </c>
+      <c r="T29" t="inlineStr">
+        <is>
+          <t>8151</t>
+        </is>
+      </c>
+      <c r="U29" t="inlineStr">
+        <is>
+          <t>67</t>
+        </is>
       </c>
     </row>
     <row r="30">
@@ -2857,7 +3125,7 @@
           <t>77:06:0008002:1155</t>
         </is>
       </c>
-      <c r="K30" s="5" t="n">
+      <c r="K30" s="11" t="n">
         <v>9</v>
       </c>
       <c r="L30" t="inlineStr">
@@ -2884,15 +3152,25 @@
           <t>8</t>
         </is>
       </c>
-      <c r="Q30" s="6">
-        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.64669_ 37.54651.json", "55.64669_ 37.54651.json")</f>
+      <c r="Q30" s="12">
+        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.64669_37.54651.json", "55.64669_37.54651.json")</f>
         <v/>
       </c>
       <c r="R30" t="n">
         <v>14560</v>
       </c>
-      <c r="S30" s="5" t="n">
+      <c r="S30" s="9" t="n">
         <v>1.66</v>
+      </c>
+      <c r="T30" t="inlineStr">
+        <is>
+          <t>2682</t>
+        </is>
+      </c>
+      <c r="U30" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
       </c>
     </row>
     <row r="31">
@@ -2937,7 +3215,7 @@
           <t>77:02:0025016:1512</t>
         </is>
       </c>
-      <c r="K31" s="5" t="n">
+      <c r="K31" s="11" t="n">
         <v>4.97</v>
       </c>
       <c r="L31" t="inlineStr">
@@ -2964,15 +3242,25 @@
           <t>42</t>
         </is>
       </c>
-      <c r="Q31" s="6">
-        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.884403_ 37.541566.json", "55.884403_ 37.541566.json")</f>
+      <c r="Q31" s="12">
+        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.884403_37.541566.json", "55.884403_37.541566.json")</f>
         <v/>
       </c>
       <c r="R31" t="n">
         <v>10093</v>
       </c>
-      <c r="S31" s="5" t="n">
+      <c r="S31" s="9" t="n">
         <v>3.89</v>
+      </c>
+      <c r="T31" t="inlineStr">
+        <is>
+          <t>7908</t>
+        </is>
+      </c>
+      <c r="U31" t="inlineStr">
+        <is>
+          <t>42</t>
+        </is>
       </c>
     </row>
     <row r="32">
@@ -3017,7 +3305,7 @@
           <t xml:space="preserve">77:09:0004011:6556, </t>
         </is>
       </c>
-      <c r="K32" s="5" t="n">
+      <c r="K32" s="11" t="n">
         <v>3.32</v>
       </c>
       <c r="L32" t="inlineStr">
@@ -3044,15 +3332,25 @@
           <t>95</t>
         </is>
       </c>
-      <c r="Q32" s="6">
-        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.797574_ 37.569468.json", "55.797574_ 37.569468.json")</f>
+      <c r="Q32" s="12">
+        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.797574_37.569468.json", "55.797574_37.569468.json")</f>
         <v/>
       </c>
       <c r="R32" t="n">
         <v>16854</v>
       </c>
-      <c r="S32" s="5" t="n">
+      <c r="S32" s="9" t="n">
         <v>2.6</v>
+      </c>
+      <c r="T32" t="inlineStr">
+        <is>
+          <t>13206</t>
+        </is>
+      </c>
+      <c r="U32" t="inlineStr">
+        <is>
+          <t>95</t>
+        </is>
       </c>
     </row>
     <row r="33">
@@ -3097,7 +3395,7 @@
           <t xml:space="preserve">77:06:0008003:1053, </t>
         </is>
       </c>
-      <c r="K33" s="5" t="n">
+      <c r="K33" s="11" t="n">
         <v>30.97</v>
       </c>
       <c r="L33" t="inlineStr">
@@ -3124,15 +3422,25 @@
           <t>45</t>
         </is>
       </c>
-      <c r="Q33" s="6">
-        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.649144_ 37.534918.json", "55.649144_ 37.534918.json")</f>
+      <c r="Q33" s="12">
+        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.649144_37.534918.json", "55.649144_37.534918.json")</f>
         <v/>
       </c>
       <c r="R33" t="n">
         <v>15589</v>
       </c>
-      <c r="S33" s="5" t="n">
+      <c r="S33" s="9" t="n">
         <v>7.97</v>
+      </c>
+      <c r="T33" t="inlineStr">
+        <is>
+          <t>4011</t>
+        </is>
+      </c>
+      <c r="U33" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
       </c>
     </row>
     <row r="34">
@@ -3177,7 +3485,7 @@
           <t>16:01:110301:4410</t>
         </is>
       </c>
-      <c r="K34" s="5" t="n">
+      <c r="K34" s="11" t="n">
         <v>18.61</v>
       </c>
       <c r="L34" t="inlineStr">
@@ -3204,15 +3512,25 @@
           <t>0</t>
         </is>
       </c>
-      <c r="Q34" s="6">
-        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/56.52616_ 52.982402.json", "56.52616_ 52.982402.json")</f>
+      <c r="Q34" s="12">
+        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/56.52616_52.982402.json", "56.52616_52.982402.json")</f>
         <v/>
       </c>
       <c r="R34" t="n">
         <v>1347</v>
       </c>
-      <c r="S34" s="5" t="n">
+      <c r="S34" s="9" t="n">
         <v>10.69</v>
+      </c>
+      <c r="T34" t="inlineStr">
+        <is>
+          <t>774</t>
+        </is>
+      </c>
+      <c r="U34" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="35">
@@ -3257,7 +3575,7 @@
           <t>58:29:3008002:4765</t>
         </is>
       </c>
-      <c r="K35" s="5" t="n">
+      <c r="K35" s="11" t="n">
         <v>6.44</v>
       </c>
       <c r="L35" t="inlineStr">
@@ -3284,15 +3602,25 @@
           <t>13</t>
         </is>
       </c>
-      <c r="Q35" s="6">
-        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/53.132946_ 45.015263.json", "53.132946_ 45.015263.json")</f>
+      <c r="Q35" s="12">
+        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/53.132946_45.015263.json", "53.132946_45.015263.json")</f>
         <v/>
       </c>
       <c r="R35" t="n">
         <v>3741</v>
       </c>
-      <c r="S35" s="5" t="n">
+      <c r="S35" s="9" t="n">
         <v>8.449999999999999</v>
+      </c>
+      <c r="T35" t="inlineStr">
+        <is>
+          <t>4911</t>
+        </is>
+      </c>
+      <c r="U35" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
       </c>
     </row>
     <row r="36">
@@ -3332,7 +3660,7 @@
           <t>11 08 22 20:59</t>
         </is>
       </c>
-      <c r="K36" s="5" t="n">
+      <c r="K36" s="11" t="n">
         <v>6.39</v>
       </c>
       <c r="L36" t="inlineStr">
@@ -3359,15 +3687,25 @@
           <t>4</t>
         </is>
       </c>
-      <c r="Q36" s="6">
-        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/56.1064309_ 47.4447934.json", "56.1064309_ 47.4447934.json")</f>
+      <c r="Q36" s="12">
+        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/56.1064309_47.4447934.json", "56.1064309_47.4447934.json")</f>
         <v/>
       </c>
       <c r="R36" t="n">
         <v>5042</v>
       </c>
-      <c r="S36" s="5" t="n">
+      <c r="S36" s="9" t="n">
         <v>5.3</v>
+      </c>
+      <c r="T36" t="inlineStr">
+        <is>
+          <t>4188</t>
+        </is>
+      </c>
+      <c r="U36" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
       </c>
     </row>
     <row r="37">
@@ -3412,7 +3750,7 @@
           <t>50:16:0402019:595</t>
         </is>
       </c>
-      <c r="K37" s="5" t="n">
+      <c r="K37" s="11" t="n">
         <v>62.56</v>
       </c>
       <c r="L37" t="inlineStr">
@@ -3439,15 +3777,25 @@
           <t>18</t>
         </is>
       </c>
-      <c r="Q37" s="6">
-        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.83291_ 38.478302.json", "55.83291_ 38.478302.json")</f>
+      <c r="Q37" s="12">
+        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.83291_38.478302.json", "55.83291_38.478302.json")</f>
         <v/>
       </c>
       <c r="R37" t="n">
         <v>861</v>
       </c>
-      <c r="S37" s="5" t="n">
+      <c r="S37" s="9" t="n">
         <v>62.78</v>
+      </c>
+      <c r="T37" t="inlineStr">
+        <is>
+          <t>864</t>
+        </is>
+      </c>
+      <c r="U37" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
       </c>
     </row>
     <row r="38">
@@ -3492,7 +3840,7 @@
           <t>50:16:0301004:2950</t>
         </is>
       </c>
-      <c r="K38" s="5" t="n">
+      <c r="K38" s="11" t="n">
         <v>22.81</v>
       </c>
       <c r="L38" t="inlineStr">
@@ -3519,15 +3867,25 @@
           <t>13</t>
         </is>
       </c>
-      <c r="Q38" s="6">
-        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.889523_ 38.48255.json", "55.889523_ 38.48255.json")</f>
+      <c r="Q38" s="12">
+        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.889523_38.48255.json", "55.889523_38.48255.json")</f>
         <v/>
       </c>
       <c r="R38" t="n">
         <v>745</v>
       </c>
-      <c r="S38" s="5" t="n">
+      <c r="S38" s="9" t="n">
         <v>74.18000000000001</v>
+      </c>
+      <c r="T38" t="inlineStr">
+        <is>
+          <t>2423</t>
+        </is>
+      </c>
+      <c r="U38" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
       </c>
     </row>
     <row r="39">
@@ -3572,7 +3930,7 @@
           <t>50:16:0302008:3674</t>
         </is>
       </c>
-      <c r="K39" s="5" t="n">
+      <c r="K39" s="11" t="n">
         <v>17.59</v>
       </c>
       <c r="L39" t="inlineStr">
@@ -3599,15 +3957,25 @@
           <t>17</t>
         </is>
       </c>
-      <c r="Q39" s="6">
-        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.844337_ 38.414143.json", "55.844337_ 38.414143.json")</f>
+      <c r="Q39" s="12">
+        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.844337_38.414143.json", "55.844337_38.414143.json")</f>
         <v/>
       </c>
       <c r="R39" t="n">
         <v>740</v>
       </c>
-      <c r="S39" s="5" t="n">
+      <c r="S39" s="9" t="n">
         <v>43.81</v>
+      </c>
+      <c r="T39" t="inlineStr">
+        <is>
+          <t>1843</t>
+        </is>
+      </c>
+      <c r="U39" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
       </c>
     </row>
     <row r="40">
@@ -3652,7 +4020,7 @@
           <t>50:16:0000000:67459</t>
         </is>
       </c>
-      <c r="K40" s="5" t="n">
+      <c r="K40" s="11" t="n">
         <v>21.26</v>
       </c>
       <c r="L40" t="inlineStr">
@@ -3679,15 +4047,25 @@
           <t>16</t>
         </is>
       </c>
-      <c r="Q40" s="6">
-        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.878666_ 38.43054.json", "55.878666_ 38.43054.json")</f>
+      <c r="Q40" s="12">
+        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.878666_38.43054.json", "55.878666_38.43054.json")</f>
         <v/>
       </c>
       <c r="R40" t="n">
         <v>1058</v>
       </c>
-      <c r="S40" s="5" t="n">
+      <c r="S40" s="9" t="n">
         <v>53.48</v>
+      </c>
+      <c r="T40" t="inlineStr">
+        <is>
+          <t>2661</t>
+        </is>
+      </c>
+      <c r="U40" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
       </c>
     </row>
     <row r="41">
@@ -3732,7 +4110,7 @@
           <t>50:16:0602003:7604</t>
         </is>
       </c>
-      <c r="K41" s="5" t="n">
+      <c r="K41" s="11" t="n">
         <v>10.11</v>
       </c>
       <c r="L41" t="inlineStr">
@@ -3759,15 +4137,25 @@
           <t>48</t>
         </is>
       </c>
-      <c r="Q41" s="6">
-        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.807157_ 38.166847.json", "55.807157_ 38.166847.json")</f>
+      <c r="Q41" s="12">
+        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.807157_38.166847.json", "55.807157_38.166847.json")</f>
         <v/>
       </c>
       <c r="R41" t="n">
         <v>1119</v>
       </c>
-      <c r="S41" s="5" t="n">
+      <c r="S41" s="9" t="n">
         <v>27.56</v>
+      </c>
+      <c r="T41" t="inlineStr">
+        <is>
+          <t>3051</t>
+        </is>
+      </c>
+      <c r="U41" t="inlineStr">
+        <is>
+          <t>48</t>
+        </is>
       </c>
     </row>
     <row r="42">
@@ -3812,7 +4200,7 @@
           <t>50:16:0000000:66901</t>
         </is>
       </c>
-      <c r="K42" s="5" t="n">
+      <c r="K42" s="11" t="n">
         <v>11.37</v>
       </c>
       <c r="L42" t="inlineStr">
@@ -3839,15 +4227,25 @@
           <t>15</t>
         </is>
       </c>
-      <c r="Q42" s="6">
-        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.877705_ 38.431175.json", "55.877705_ 38.431175.json")</f>
+      <c r="Q42" s="12">
+        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.877705_38.431175.json", "55.877705_38.431175.json")</f>
         <v/>
       </c>
       <c r="R42" t="n">
         <v>1058</v>
       </c>
-      <c r="S42" s="5" t="n">
+      <c r="S42" s="9" t="n">
         <v>33.63</v>
+      </c>
+      <c r="T42" t="inlineStr">
+        <is>
+          <t>3129</t>
+        </is>
+      </c>
+      <c r="U42" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
       </c>
     </row>
     <row r="43">
@@ -3892,7 +4290,7 @@
           <t>50:43:0020301:649</t>
         </is>
       </c>
-      <c r="K43" s="5" t="n">
+      <c r="K43" s="11" t="n">
         <v>10.56</v>
       </c>
       <c r="L43" t="inlineStr">
@@ -3919,15 +4317,25 @@
           <t>44</t>
         </is>
       </c>
-      <c r="Q43" s="6">
-        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.967567_ 37.916163.json", "55.967567_ 37.916163.json")</f>
+      <c r="Q43" s="12">
+        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.967567_37.916163.json", "55.967567_37.916163.json")</f>
         <v/>
       </c>
       <c r="R43" t="n">
         <v>4343</v>
       </c>
-      <c r="S43" s="5" t="n">
+      <c r="S43" s="9" t="n">
         <v>8.93</v>
+      </c>
+      <c r="T43" t="inlineStr">
+        <is>
+          <t>3675</t>
+        </is>
+      </c>
+      <c r="U43" t="inlineStr">
+        <is>
+          <t>44</t>
+        </is>
       </c>
     </row>
     <row r="44">
@@ -3972,7 +4380,7 @@
           <t>77:09:0001020:2318</t>
         </is>
       </c>
-      <c r="K44" s="5" t="n">
+      <c r="K44" s="11" t="n">
         <v>4.43</v>
       </c>
       <c r="L44" t="inlineStr">
@@ -3999,15 +4407,25 @@
           <t>45</t>
         </is>
       </c>
-      <c r="Q44" s="6">
-        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.84495_ 37.481523.json", "55.84495_ 37.481523.json")</f>
+      <c r="Q44" s="12">
+        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.84495_37.481523.json", "55.84495_37.481523.json")</f>
         <v/>
       </c>
       <c r="R44" t="n">
         <v>8383</v>
       </c>
-      <c r="S44" s="5" t="n">
+      <c r="S44" s="9" t="n">
         <v>4.45</v>
+      </c>
+      <c r="T44" t="inlineStr">
+        <is>
+          <t>8418</t>
+        </is>
+      </c>
+      <c r="U44" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
       </c>
     </row>
     <row r="45">
@@ -4052,7 +4470,7 @@
           <t>77:09:0003013:2544</t>
         </is>
       </c>
-      <c r="K45" s="5" t="n">
+      <c r="K45" s="11" t="n">
         <v>10.83</v>
       </c>
       <c r="L45" t="inlineStr">
@@ -4079,15 +4497,25 @@
           <t>182</t>
         </is>
       </c>
-      <c r="Q45" s="6">
-        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.817997_ 37.50125.json", "55.817997_ 37.50125.json")</f>
+      <c r="Q45" s="12">
+        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.817997_37.50125.json", "55.817997_37.50125.json")</f>
         <v/>
       </c>
       <c r="R45" t="n">
         <v>9085</v>
       </c>
-      <c r="S45" s="5" t="n">
+      <c r="S45" s="9" t="n">
         <v>6.79</v>
+      </c>
+      <c r="T45" t="inlineStr">
+        <is>
+          <t>5694</t>
+        </is>
+      </c>
+      <c r="U45" t="inlineStr">
+        <is>
+          <t>182</t>
+        </is>
       </c>
     </row>
     <row r="46">
@@ -4132,7 +4560,7 @@
           <t>77:04:0001019:9656</t>
         </is>
       </c>
-      <c r="K46" s="5" t="n">
+      <c r="K46" s="11" t="n">
         <v>5.84</v>
       </c>
       <c r="L46" t="inlineStr">
@@ -4159,15 +4587,25 @@
           <t>57</t>
         </is>
       </c>
-      <c r="Q46" s="6">
-        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.72636_ 37.671049.json", "55.72636_ 37.671049.json")</f>
+      <c r="Q46" s="12">
+        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.72636_37.671049.json", "55.72636_37.671049.json")</f>
         <v/>
       </c>
       <c r="R46" t="n">
         <v>10557</v>
       </c>
-      <c r="S46" s="5" t="n">
+      <c r="S46" s="9" t="n">
         <v>4.67</v>
+      </c>
+      <c r="T46" t="inlineStr">
+        <is>
+          <t>8451</t>
+        </is>
+      </c>
+      <c r="U46" t="inlineStr">
+        <is>
+          <t>57</t>
+        </is>
       </c>
     </row>
     <row r="47">
@@ -4212,7 +4650,7 @@
           <t>77:02:0010009:3795</t>
         </is>
       </c>
-      <c r="K47" s="5" t="n">
+      <c r="K47" s="11" t="n">
         <v>5.47</v>
       </c>
       <c r="L47" t="inlineStr">
@@ -4239,15 +4677,25 @@
           <t>89</t>
         </is>
       </c>
-      <c r="Q47" s="6">
-        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.872243_ 37.679323.json", "55.872243_ 37.679323.json")</f>
+      <c r="Q47" s="12">
+        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.872243_37.679323.json", "55.872243_37.679323.json")</f>
         <v/>
       </c>
       <c r="R47" t="n">
         <v>11588</v>
       </c>
-      <c r="S47" s="5" t="n">
+      <c r="S47" s="9" t="n">
         <v>2.96</v>
+      </c>
+      <c r="T47" t="inlineStr">
+        <is>
+          <t>6264</t>
+        </is>
+      </c>
+      <c r="U47" t="inlineStr">
+        <is>
+          <t>89</t>
+        </is>
       </c>
     </row>
     <row r="48">
@@ -4292,7 +4740,7 @@
           <t>50:35:0000000:20800</t>
         </is>
       </c>
-      <c r="K48" s="5" t="n">
+      <c r="K48" s="11" t="n">
         <v>11.08</v>
       </c>
       <c r="L48" t="inlineStr">
@@ -4319,15 +4767,25 @@
           <t>2</t>
         </is>
       </c>
-      <c r="Q48" s="6">
-        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/54.95581_ 39.185681.json", "54.95581_ 39.185681.json")</f>
+      <c r="Q48" s="12">
+        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/54.95581_39.185681.json", "54.95581_39.185681.json")</f>
         <v/>
       </c>
       <c r="R48" t="n">
         <v>85</v>
       </c>
-      <c r="S48" s="5" t="n">
+      <c r="S48" s="9" t="n">
         <v>116.11</v>
+      </c>
+      <c r="T48" t="inlineStr">
+        <is>
+          <t>891</t>
+        </is>
+      </c>
+      <c r="U48" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
     </row>
     <row r="49">
@@ -4372,7 +4830,7 @@
           <t>50:04:0010202:6923</t>
         </is>
       </c>
-      <c r="K49" s="5" t="n">
+      <c r="K49" s="11" t="n">
         <v>6.89</v>
       </c>
       <c r="L49" t="inlineStr">
@@ -4399,15 +4857,25 @@
           <t>13</t>
         </is>
       </c>
-      <c r="Q49" s="6">
-        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/56.341003_ 37.548286.json", "56.341003_ 37.548286.json")</f>
+      <c r="Q49" s="12">
+        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/56.341003_37.548286.json", "56.341003_37.548286.json")</f>
         <v/>
       </c>
       <c r="R49" t="n">
         <v>579</v>
       </c>
-      <c r="S49" s="5" t="n">
+      <c r="S49" s="9" t="n">
         <v>55.77</v>
+      </c>
+      <c r="T49" t="inlineStr">
+        <is>
+          <t>4686</t>
+        </is>
+      </c>
+      <c r="U49" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
       </c>
     </row>
     <row r="50">
@@ -4452,7 +4920,7 @@
           <t>50:04:0010202:6922</t>
         </is>
       </c>
-      <c r="K50" s="5" t="n">
+      <c r="K50" s="11" t="n">
         <v>6.77</v>
       </c>
       <c r="L50" t="inlineStr">
@@ -4479,15 +4947,25 @@
           <t>13</t>
         </is>
       </c>
-      <c r="Q50" s="6">
-        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/56.341003_ 37.548286.json", "56.341003_ 37.548286.json")</f>
+      <c r="Q50" s="12">
+        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/56.341003_37.548286.json", "56.341003_37.548286.json")</f>
         <v/>
       </c>
       <c r="R50" t="n">
         <v>579</v>
       </c>
-      <c r="S50" s="5" t="n">
+      <c r="S50" s="9" t="n">
         <v>54.8</v>
+      </c>
+      <c r="T50" t="inlineStr">
+        <is>
+          <t>4686</t>
+        </is>
+      </c>
+      <c r="U50" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
       </c>
     </row>
     <row r="51">
@@ -4532,7 +5010,7 @@
           <t>77:01:0001060:2215</t>
         </is>
       </c>
-      <c r="K51" s="5" t="n">
+      <c r="K51" s="11" t="n">
         <v>6.54</v>
       </c>
       <c r="L51" t="inlineStr">
@@ -4559,15 +5037,25 @@
           <t>305</t>
         </is>
       </c>
-      <c r="Q51" s="6">
-        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.748701_ 37.5857.json", "55.748701_ 37.5857.json")</f>
+      <c r="Q51" s="12">
+        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.748701_37.5857.json", "55.748701_37.5857.json")</f>
         <v/>
       </c>
       <c r="R51" t="n">
         <v>9937</v>
       </c>
-      <c r="S51" s="5" t="n">
+      <c r="S51" s="9" t="n">
         <v>10.88</v>
+      </c>
+      <c r="T51" t="inlineStr">
+        <is>
+          <t>16530</t>
+        </is>
+      </c>
+      <c r="U51" t="inlineStr">
+        <is>
+          <t>305</t>
+        </is>
       </c>
     </row>
     <row r="52">
@@ -4612,7 +5100,7 @@
           <t>77:02:0010008:4833</t>
         </is>
       </c>
-      <c r="K52" s="5" t="n">
+      <c r="K52" s="11" t="n">
         <v>3.78</v>
       </c>
       <c r="L52" t="inlineStr">
@@ -4639,15 +5127,25 @@
           <t>50</t>
         </is>
       </c>
-      <c r="Q52" s="6">
-        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.861974_ 37.676825.json", "55.861974_ 37.676825.json")</f>
+      <c r="Q52" s="12">
+        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.861974_37.676825.json", "55.861974_37.676825.json")</f>
         <v/>
       </c>
       <c r="R52" t="n">
         <v>12575</v>
       </c>
-      <c r="S52" s="5" t="n">
+      <c r="S52" s="9" t="n">
         <v>3.62</v>
+      </c>
+      <c r="T52" t="inlineStr">
+        <is>
+          <t>12051</t>
+        </is>
+      </c>
+      <c r="U52" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
       </c>
     </row>
     <row r="53">
@@ -4692,7 +5190,7 @@
           <t>77:05:0004009:13807; 77:05:0004009:13808</t>
         </is>
       </c>
-      <c r="K53" s="5" t="n">
+      <c r="K53" s="11" t="n">
         <v>9.140000000000001</v>
       </c>
       <c r="L53" t="inlineStr">
@@ -4719,15 +5217,25 @@
           <t>33</t>
         </is>
       </c>
-      <c r="Q53" s="6">
-        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.685158_ 37.68641.json", "55.685158_ 37.68641.json")</f>
+      <c r="Q53" s="12">
+        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.685158_37.68641.json", "55.685158_37.68641.json")</f>
         <v/>
       </c>
       <c r="R53" t="n">
         <v>9074</v>
       </c>
-      <c r="S53" s="5" t="n">
+      <c r="S53" s="9" t="n">
         <v>9.26</v>
+      </c>
+      <c r="T53" t="inlineStr">
+        <is>
+          <t>9192</t>
+        </is>
+      </c>
+      <c r="U53" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
       </c>
     </row>
     <row r="54">
@@ -4830,7 +5338,7 @@
           <t>77:03:0006014:3030</t>
         </is>
       </c>
-      <c r="K55" s="5" t="n">
+      <c r="K55" s="11" t="n">
         <v>16.58</v>
       </c>
       <c r="L55" t="inlineStr">
@@ -4857,15 +5365,25 @@
           <t>28</t>
         </is>
       </c>
-      <c r="Q55" s="6">
-        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.613916_ 37.494368.json", "55.613916_ 37.494368.json")</f>
+      <c r="Q55" s="12">
+        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.613916_37.494368.json", "55.613916_37.494368.json")</f>
         <v/>
       </c>
       <c r="R55" t="n">
         <v>5819</v>
       </c>
-      <c r="S55" s="5" t="n">
+      <c r="S55" s="9" t="n">
         <v>7.31</v>
+      </c>
+      <c r="T55" t="inlineStr">
+        <is>
+          <t>2565</t>
+        </is>
+      </c>
+      <c r="U55" t="inlineStr">
+        <is>
+          <t>28</t>
+        </is>
       </c>
     </row>
     <row r="56">
@@ -4910,7 +5428,7 @@
           <t>50:46:0010502:1775</t>
         </is>
       </c>
-      <c r="K56" s="5" t="n">
+      <c r="K56" s="11" t="n">
         <v>6.41</v>
       </c>
       <c r="L56" t="inlineStr">
@@ -4937,15 +5455,25 @@
           <t>36</t>
         </is>
       </c>
-      <c r="Q56" s="6">
-        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.796005_ 38.443806.json", "55.796005_ 38.443806.json")</f>
+      <c r="Q56" s="12">
+        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.796005_38.443806.json", "55.796005_38.443806.json")</f>
         <v/>
       </c>
       <c r="R56" t="n">
         <v>4449</v>
       </c>
-      <c r="S56" s="5" t="n">
+      <c r="S56" s="9" t="n">
         <v>6.01</v>
+      </c>
+      <c r="T56" t="inlineStr">
+        <is>
+          <t>4170</t>
+        </is>
+      </c>
+      <c r="U56" t="inlineStr">
+        <is>
+          <t>36</t>
+        </is>
       </c>
     </row>
     <row r="57">
@@ -4990,7 +5518,7 @@
           <t>50:46:0000000:5133</t>
         </is>
       </c>
-      <c r="K57" s="5" t="n">
+      <c r="K57" s="11" t="n">
         <v>52.44</v>
       </c>
       <c r="L57" t="inlineStr">
@@ -5017,15 +5545,25 @@
           <t>51</t>
         </is>
       </c>
-      <c r="Q57" s="6">
-        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.79628_ 38.466183.json", "55.79628_ 38.466183.json")</f>
+      <c r="Q57" s="12">
+        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.79628_38.466183.json", "55.79628_38.466183.json")</f>
         <v/>
       </c>
       <c r="R57" t="n">
         <v>4323</v>
       </c>
-      <c r="S57" s="5" t="n">
+      <c r="S57" s="9" t="n">
         <v>5.71</v>
+      </c>
+      <c r="T57" t="inlineStr">
+        <is>
+          <t>471</t>
+        </is>
+      </c>
+      <c r="U57" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
       </c>
     </row>
     <row r="58">
@@ -5070,7 +5608,7 @@
           <t>77:05:0002006:4951</t>
         </is>
       </c>
-      <c r="K58" s="5" t="n">
+      <c r="K58" s="11" t="n">
         <v>3.96</v>
       </c>
       <c r="L58" t="inlineStr">
@@ -5097,15 +5635,25 @@
           <t>73</t>
         </is>
       </c>
-      <c r="Q58" s="6">
-        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.705047_ 37.669001.json", "55.705047_ 37.669001.json")</f>
+      <c r="Q58" s="12">
+        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.705047_37.669001.json", "55.705047_37.669001.json")</f>
         <v/>
       </c>
       <c r="R58" t="n">
         <v>9152</v>
       </c>
-      <c r="S58" s="5" t="n">
+      <c r="S58" s="9" t="n">
         <v>5.47</v>
+      </c>
+      <c r="T58" t="inlineStr">
+        <is>
+          <t>12633</t>
+        </is>
+      </c>
+      <c r="U58" t="inlineStr">
+        <is>
+          <t>73</t>
+        </is>
       </c>
     </row>
     <row r="59">
@@ -5150,7 +5698,7 @@
           <t>77:06:0001006:3792</t>
         </is>
       </c>
-      <c r="K59" s="5" t="n">
+      <c r="K59" s="11" t="n">
         <v>6.64</v>
       </c>
       <c r="L59" t="inlineStr">
@@ -5177,15 +5725,25 @@
           <t>107</t>
         </is>
       </c>
-      <c r="Q59" s="6">
-        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.67855_ 37.526276.json", "55.67855_ 37.526276.json")</f>
+      <c r="Q59" s="12">
+        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.67855_37.526276.json", "55.67855_37.526276.json")</f>
         <v/>
       </c>
       <c r="R59" t="n">
         <v>22860</v>
       </c>
-      <c r="S59" s="5" t="n">
+      <c r="S59" s="9" t="n">
         <v>1.73</v>
+      </c>
+      <c r="T59" t="inlineStr">
+        <is>
+          <t>5970</t>
+        </is>
+      </c>
+      <c r="U59" t="inlineStr">
+        <is>
+          <t>107</t>
+        </is>
       </c>
     </row>
     <row r="60">
@@ -5230,7 +5788,7 @@
           <t>77:03:0005004:5095</t>
         </is>
       </c>
-      <c r="K60" s="5" t="n">
+      <c r="K60" s="11" t="n">
         <v>5.71</v>
       </c>
       <c r="L60" t="inlineStr">
@@ -5257,15 +5815,25 @@
           <t>123</t>
         </is>
       </c>
-      <c r="Q60" s="6">
-        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.792716_ 37.780194.json", "55.792716_ 37.780194.json")</f>
+      <c r="Q60" s="12">
+        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.792716_37.780194.json", "55.792716_37.780194.json")</f>
         <v/>
       </c>
       <c r="R60" t="n">
         <v>6258</v>
       </c>
-      <c r="S60" s="5" t="n">
+      <c r="S60" s="9" t="n">
         <v>11.12</v>
+      </c>
+      <c r="T60" t="inlineStr">
+        <is>
+          <t>12186</t>
+        </is>
+      </c>
+      <c r="U60" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
       </c>
     </row>
     <row r="61">
@@ -5310,7 +5878,7 @@
           <t>77:03:0005004:5089, 77:03:0005004:5093</t>
         </is>
       </c>
-      <c r="K61" s="5" t="n">
+      <c r="K61" s="11" t="n">
         <v>4.88</v>
       </c>
       <c r="L61" t="inlineStr">
@@ -5337,15 +5905,25 @@
           <t>123</t>
         </is>
       </c>
-      <c r="Q61" s="6">
-        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.792716_ 37.780194.json", "55.792716_ 37.780194.json")</f>
+      <c r="Q61" s="12">
+        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.792716_37.780194.json", "55.792716_37.780194.json")</f>
         <v/>
       </c>
       <c r="R61" t="n">
         <v>6258</v>
       </c>
-      <c r="S61" s="5" t="n">
+      <c r="S61" s="9" t="n">
         <v>9.51</v>
+      </c>
+      <c r="T61" t="inlineStr">
+        <is>
+          <t>12186</t>
+        </is>
+      </c>
+      <c r="U61" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
       </c>
     </row>
     <row r="62">
@@ -5390,7 +5968,7 @@
           <t>50:17:0021502:30</t>
         </is>
       </c>
-      <c r="K62" s="5" t="n">
+      <c r="K62" s="11" t="n">
         <v>4.88</v>
       </c>
       <c r="L62" t="inlineStr">
@@ -5417,15 +5995,25 @@
           <t>30</t>
         </is>
       </c>
-      <c r="Q62" s="6">
-        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.77192_ 38.656456.json", "55.77192_ 38.656456.json")</f>
+      <c r="Q62" s="12">
+        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.77192_38.656456.json", "55.77192_38.656456.json")</f>
         <v/>
       </c>
       <c r="R62" t="n">
         <v>1304</v>
       </c>
-      <c r="S62" s="5" t="n">
+      <c r="S62" s="9" t="n">
         <v>10.64</v>
+      </c>
+      <c r="T62" t="inlineStr">
+        <is>
+          <t>2841</t>
+        </is>
+      </c>
+      <c r="U62" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
       </c>
     </row>
     <row r="63">
@@ -5470,7 +6058,7 @@
           <t>77:03:0005008:7128</t>
         </is>
       </c>
-      <c r="K63" s="5" t="n">
+      <c r="K63" s="11" t="n">
         <v>3.78</v>
       </c>
       <c r="L63" t="inlineStr">
@@ -5497,15 +6085,25 @@
           <t>40</t>
         </is>
       </c>
-      <c r="Q63" s="6">
-        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.800013_ 37.804844.json", "55.800013_ 37.804844.json")</f>
+      <c r="Q63" s="12">
+        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.800013_37.804844.json", "55.800013_37.804844.json")</f>
         <v/>
       </c>
       <c r="R63" t="n">
         <v>9319</v>
       </c>
-      <c r="S63" s="5" t="n">
+      <c r="S63" s="9" t="n">
         <v>4.44</v>
+      </c>
+      <c r="T63" t="inlineStr">
+        <is>
+          <t>10941</t>
+        </is>
+      </c>
+      <c r="U63" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
       </c>
     </row>
     <row r="64">
@@ -5550,7 +6148,7 @@
           <t>77:03:0003003:2242</t>
         </is>
       </c>
-      <c r="K64" s="5" t="n">
+      <c r="K64" s="11" t="n">
         <v>8.779999999999999</v>
       </c>
       <c r="L64" t="inlineStr">
@@ -5577,15 +6175,25 @@
           <t>91</t>
         </is>
       </c>
-      <c r="Q64" s="6">
-        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.79057_ 37.668148.json", "55.79057_ 37.668148.json")</f>
+      <c r="Q64" s="12">
+        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.79057_37.668148.json", "55.79057_37.668148.json")</f>
         <v/>
       </c>
       <c r="R64" t="n">
         <v>4877</v>
       </c>
-      <c r="S64" s="5" t="n">
+      <c r="S64" s="9" t="n">
         <v>16.48</v>
+      </c>
+      <c r="T64" t="inlineStr">
+        <is>
+          <t>9154</t>
+        </is>
+      </c>
+      <c r="U64" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
       </c>
     </row>
     <row r="65">
@@ -5630,7 +6238,7 @@
           <t>77:04:0005004:8881</t>
         </is>
       </c>
-      <c r="K65" s="5" t="n">
+      <c r="K65" s="11" t="n">
         <v>19.9</v>
       </c>
       <c r="L65" t="inlineStr">
@@ -5657,15 +6265,25 @@
           <t>147</t>
         </is>
       </c>
-      <c r="Q65" s="6">
-        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.677854_ 37.857.json", "55.677854_ 37.857.json")</f>
+      <c r="Q65" s="12">
+        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.677854_37.857.json", "55.677854_37.857.json")</f>
         <v/>
       </c>
       <c r="R65" t="n">
         <v>3969</v>
       </c>
-      <c r="S65" s="5" t="n">
+      <c r="S65" s="9" t="n">
         <v>36.26</v>
+      </c>
+      <c r="T65" t="inlineStr">
+        <is>
+          <t>7233</t>
+        </is>
+      </c>
+      <c r="U65" t="inlineStr">
+        <is>
+          <t>147</t>
+        </is>
       </c>
     </row>
     <row r="66">
@@ -5710,7 +6328,7 @@
           <t>77:03:0003003:2243</t>
         </is>
       </c>
-      <c r="K66" s="5" t="n">
+      <c r="K66" s="11" t="n">
         <v>8.77</v>
       </c>
       <c r="L66" t="inlineStr">
@@ -5737,15 +6355,25 @@
           <t>91</t>
         </is>
       </c>
-      <c r="Q66" s="6">
-        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.79057_ 37.668148.json", "55.79057_ 37.668148.json")</f>
+      <c r="Q66" s="12">
+        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.79057_37.668148.json", "55.79057_37.668148.json")</f>
         <v/>
       </c>
       <c r="R66" t="n">
         <v>4877</v>
       </c>
-      <c r="S66" s="5" t="n">
+      <c r="S66" s="9" t="n">
         <v>16.45</v>
+      </c>
+      <c r="T66" t="inlineStr">
+        <is>
+          <t>9154</t>
+        </is>
+      </c>
+      <c r="U66" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
       </c>
     </row>
     <row r="67">
@@ -5790,7 +6418,7 @@
           <t>77:03:0003017:4070</t>
         </is>
       </c>
-      <c r="K67" s="5" t="n">
+      <c r="K67" s="11" t="n">
         <v>14.79</v>
       </c>
       <c r="L67" t="inlineStr">
@@ -5817,15 +6445,25 @@
           <t>68</t>
         </is>
       </c>
-      <c r="Q67" s="6">
-        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.78359_ 37.727894.json", "55.78359_ 37.727894.json")</f>
+      <c r="Q67" s="12">
+        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.78359_37.727894.json", "55.78359_37.727894.json")</f>
         <v/>
       </c>
       <c r="R67" t="n">
         <v>8854</v>
       </c>
-      <c r="S67" s="5" t="n">
+      <c r="S67" s="9" t="n">
         <v>12.33</v>
+      </c>
+      <c r="T67" t="inlineStr">
+        <is>
+          <t>7386</t>
+        </is>
+      </c>
+      <c r="U67" t="inlineStr">
+        <is>
+          <t>68</t>
+        </is>
       </c>
     </row>
     <row r="68">
@@ -5870,7 +6508,7 @@
           <t>77:09:0005003:6567</t>
         </is>
       </c>
-      <c r="K68" s="5" t="n">
+      <c r="K68" s="11" t="n">
         <v>6.25</v>
       </c>
       <c r="L68" t="inlineStr">
@@ -5897,15 +6535,25 @@
           <t>109</t>
         </is>
       </c>
-      <c r="Q68" s="6">
-        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.795406_ 37.512543.json", "55.795406_ 37.512543.json")</f>
+      <c r="Q68" s="12">
+        <f>HYPERLINK("D:\torgi_project\venv_torgi\objs_in_district/55.795406_37.512543.json", "55.795406_37.512543.json")</f>
         <v/>
       </c>
       <c r="R68" t="n">
         <v>10376</v>
       </c>
-      <c r="S68" s="5" t="n">
+      <c r="S68" s="9" t="n">
         <v>7.66</v>
+      </c>
+      <c r="T68" t="inlineStr">
+        <is>
+          <t>12708</t>
+        </is>
+      </c>
+      <c r="U68" t="inlineStr">
+        <is>
+          <t>109</t>
+        </is>
       </c>
     </row>
     <row r="69">
@@ -6083,12 +6731,15 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B100"/>
+  <autoFilter ref="A1:B100">
+    <filterColumn colId="1"/>
+  </autoFilter>
   <conditionalFormatting sqref="L1:L1000">
     <cfRule type="containsText" priority="1" operator="containsText" dxfId="0" text="PP">
       <formula>NOT(ISERROR(SEARCH("PP",L1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" paperSize="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>